<commit_message>
upgraded titration barrel recipe serialisation
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\final_beverage_recipes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9CF027-0256-42CF-A5A3-20249B749E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8B8C8C-8017-4F18-963E-D86EF4E9757E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -547,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="B1">
-        <v>0.08</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -736,51 +736,51 @@
       </c>
       <c r="B8" s="13">
         <f>$B$1</f>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="C8" s="13">
         <f t="shared" ref="C8:M8" si="0">$B$1</f>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="D8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="E8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="F8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="H8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="I8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="J8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="K8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="L8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
       <c r="M8" s="13">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -842,51 +842,51 @@
       </c>
       <c r="B10" s="2">
         <f>IF(B8=0,0,LOG((0.5+B3/2)*B9*(0.5+B5/2),1+B8)/100)</f>
-        <v>0.41928278865273511</v>
+        <v>4.6553518286125542E-2</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" ref="C10:M10" si="2">IF(C8=0,0,LOG((0.5+C3/2)*C9*(0.5+C5/2),1+C8)/100)</f>
-        <v>0.59941215549274685</v>
+        <v>6.6553518286125546E-2</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>0.65209661793277274</v>
+        <v>7.2403143293337108E-2</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>0.86960620575276448</v>
+        <v>9.6553518286125545E-2</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="2"/>
-        <v>0.95967088917277044</v>
+        <v>0.10655351828612554</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="2"/>
-        <v>1.0497355725927762</v>
+        <v>0.11655351828612556</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="2"/>
-        <v>1.1398002560127822</v>
+        <v>0.12655351828612557</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="2"/>
-        <v>0.509347472072741</v>
+        <v>5.6553518286125544E-2</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="2"/>
-        <v>0.509347472072741</v>
+        <v>5.6553518286125544E-2</v>
       </c>
       <c r="K10" s="2">
         <f t="shared" si="2"/>
-        <v>0.509347472072741</v>
+        <v>5.6553518286125544E-2</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" si="2"/>
-        <v>0.509347472072741</v>
+        <v>5.6553518286125544E-2</v>
       </c>
       <c r="M10" s="2">
         <f t="shared" si="2"/>
-        <v>0.509347472072741</v>
+        <v>5.6553518286125544E-2</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
moved matchIngredientStacksExclusively into GatedSpectrumRecipe
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A283CA87-34DA-4F9A-82A4-0C31AB9CFDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E12F744-4D2F-4B1A-8312-B3259D7E93EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34395" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>this is noted in the resulting items tooltip</t>
   </si>
   <si>
-    <t>player has the choice to add less / more input items than required in the recipe. More items than required results in thickness &gt; 1</t>
-  </si>
-  <si>
     <t>higher fermentation time &amp; thickness result in higher alc %, heavily influenced by the fermentation mod</t>
   </si>
   <si>
@@ -95,7 +92,10 @@
     <t>The real life hours the player had the barrel sealed before tapping</t>
   </si>
   <si>
-    <t>The total amount of ingredients put into the barrel. Does not need to match "recipe ingredient #"</t>
+    <t>The total amount of ingredients put into the barrel. Has to be &gt;= "recipe ingredient #"</t>
+  </si>
+  <si>
+    <t>player has the choice to add more input items than required in the recipe. More items than required results in a thickness &gt; 1</t>
   </si>
 </sst>
 </file>
@@ -696,7 +696,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -721,7 +721,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -733,7 +733,7 @@
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4"/>
       <c r="F4"/>
@@ -818,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -862,7 +862,7 @@
         <v>72</v>
       </c>
       <c r="O8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -906,7 +906,7 @@
         <v>0.4</v>
       </c>
       <c r="O9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -1050,7 +1050,7 @@
         <v>1.5</v>
       </c>
       <c r="O13" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1106,7 +1106,7 @@
         <v>7.5622424242210731E-2</v>
       </c>
       <c r="O14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1114,55 +1114,55 @@
         <v>6</v>
       </c>
       <c r="B15" s="38">
-        <f>ABS(0.5+B13/2)</f>
+        <f t="shared" ref="B15:M15" si="3">ABS(0.5+B13/2)</f>
         <v>1</v>
       </c>
       <c r="C15" s="22">
-        <f>ABS(0.5+C13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="D15" s="22">
-        <f>ABS(0.5+D13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="E15" s="22">
-        <f>ABS(0.5+E13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="F15" s="22">
-        <f>ABS(0.5+F13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="G15" s="22">
-        <f>ABS(0.5+G13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="H15" s="22">
-        <f>ABS(0.5+H13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="I15" s="22">
-        <f>ABS(0.5+I13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="J15" s="22">
-        <f>ABS(0.5+J13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="K15" s="22">
-        <f>ABS(0.5+K13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="L15" s="22">
-        <f>ABS(0.5+L13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="M15" s="23">
-        <f>ABS(0.5+M13/2)</f>
+        <f t="shared" si="3"/>
         <v>1.25</v>
       </c>
       <c r="O15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
standardised beverage fermentation times
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2787D400-174A-40F3-9B4C-A93191670F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D85C27-8480-4A0D-8587-B88785C631A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21360" yWindow="0" windowWidth="30240" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34395" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="137">
   <si>
     <t>thickness</t>
   </si>
@@ -96,6 +96,354 @@
   </si>
   <si>
     <t>player has the choice to add more input items than required in the recipe. More items than required results in a thickness &gt; 1</t>
+  </si>
+  <si>
+    <t>Beer</t>
+  </si>
+  <si>
+    <t>High %</t>
+  </si>
+  <si>
+    <t>Beverage Type</t>
+  </si>
+  <si>
+    <t>4 days</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>Downfall:</t>
+  </si>
+  <si>
+    <t>Thickness:</t>
+  </si>
+  <si>
+    <t>1/2 day</t>
+  </si>
+  <si>
+    <t>1 day</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>1 month</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>576</t>
+  </si>
+  <si>
+    <t>720</t>
+  </si>
+  <si>
+    <t>beer, ale, lager, porter</t>
+  </si>
+  <si>
+    <t>malt_beer</t>
+  </si>
+  <si>
+    <t>Cider</t>
+  </si>
+  <si>
+    <t>apple_cider</t>
+  </si>
+  <si>
+    <t>apple_cider, berry_cider, glow_berry_cider</t>
+  </si>
+  <si>
+    <t>Liquor / Creme Liquor</t>
+  </si>
+  <si>
+    <t>gin, rum, tequilla, vodka, mint_schnapps, rabbit_poison, damassine</t>
+  </si>
+  <si>
+    <t>Golden Apple Cider</t>
+  </si>
+  <si>
+    <t>Enchanted Apple Cider</t>
+  </si>
+  <si>
+    <t>Moonshine</t>
+  </si>
+  <si>
+    <t>Reprise</t>
+  </si>
+  <si>
+    <t>Entries:</t>
+  </si>
+  <si>
+    <t>"well known" fermentation mods</t>
+  </si>
+  <si>
+    <t>Ferm.Mod</t>
+  </si>
+  <si>
+    <t>Min Time (h)</t>
+  </si>
+  <si>
+    <t>Jade Wine</t>
+  </si>
+  <si>
+    <t>Suspicious Brew</t>
+  </si>
+  <si>
+    <t>(nectar multiplies days by 1.5 and dampens negative effects)</t>
+  </si>
+  <si>
+    <t>berry_liquor, glow_berry_liquor, advocaat, mint_cream, hare_bane_creme, incubus_cream, mead, artemisa</t>
+  </si>
+  <si>
+    <t>Non Alcoholic</t>
+  </si>
+  <si>
+    <t>beer</t>
+  </si>
+  <si>
+    <t>ale</t>
+  </si>
+  <si>
+    <t>lager</t>
+  </si>
+  <si>
+    <t>porter</t>
+  </si>
+  <si>
+    <t>berry_cider</t>
+  </si>
+  <si>
+    <t>glow_berry_cider</t>
+  </si>
+  <si>
+    <t>berry_liquor</t>
+  </si>
+  <si>
+    <t>glow_berry_liquor</t>
+  </si>
+  <si>
+    <t>advocaat</t>
+  </si>
+  <si>
+    <t>mint_cream</t>
+  </si>
+  <si>
+    <t>hare_bane_creme</t>
+  </si>
+  <si>
+    <t>incubus_cream</t>
+  </si>
+  <si>
+    <t>mead</t>
+  </si>
+  <si>
+    <t>artemisa</t>
+  </si>
+  <si>
+    <t>gin</t>
+  </si>
+  <si>
+    <t>rum</t>
+  </si>
+  <si>
+    <t>tequilla</t>
+  </si>
+  <si>
+    <t>vodka</t>
+  </si>
+  <si>
+    <t>mint_schnapps</t>
+  </si>
+  <si>
+    <t>rabbit_poison</t>
+  </si>
+  <si>
+    <t>damassine</t>
+  </si>
+  <si>
+    <t>golden_apple_cider</t>
+  </si>
+  <si>
+    <t>enchanted_apple_cider</t>
+  </si>
+  <si>
+    <t>moonshine</t>
+  </si>
+  <si>
+    <t>nourishing</t>
+  </si>
+  <si>
+    <t>saturation</t>
+  </si>
+  <si>
+    <t>nausea</t>
+  </si>
+  <si>
+    <t>slowness</t>
+  </si>
+  <si>
+    <t>health_boost</t>
+  </si>
+  <si>
+    <t>blindness</t>
+  </si>
+  <si>
+    <t>haste</t>
+  </si>
+  <si>
+    <t>regeneration</t>
+  </si>
+  <si>
+    <t>resistance</t>
+  </si>
+  <si>
+    <t>wheat, sweet_berries, sugar_cane</t>
+  </si>
+  <si>
+    <t>wheat</t>
+  </si>
+  <si>
+    <t>wheat, honey_bottle</t>
+  </si>
+  <si>
+    <t>wheat, wheat_seeds, beetroot</t>
+  </si>
+  <si>
+    <t>wheat, sugar</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>swiftness</t>
+  </si>
+  <si>
+    <t>glowing</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>sweet_berries</t>
+  </si>
+  <si>
+    <t>glow_berries</t>
+  </si>
+  <si>
+    <t>sweet_berries, sugar</t>
+  </si>
+  <si>
+    <t>glow_berries, sugar</t>
+  </si>
+  <si>
+    <t>potato, mermaids_gem, four_leaf_clover, sugar, snowball</t>
+  </si>
+  <si>
+    <t>carrow, sugar</t>
+  </si>
+  <si>
+    <t>another_roll</t>
+  </si>
+  <si>
+    <t>luck</t>
+  </si>
+  <si>
+    <t>jump_boost</t>
+  </si>
+  <si>
+    <t>honey_bottle</t>
+  </si>
+  <si>
+    <t>fire_resistance</t>
+  </si>
+  <si>
+    <t>grass, fern, sugar</t>
+  </si>
+  <si>
+    <t>poison</t>
+  </si>
+  <si>
+    <t>unluck</t>
+  </si>
+  <si>
+    <t>blazing</t>
+  </si>
+  <si>
+    <t>crimson_fungus, weeping_vines, clotted_cream</t>
+  </si>
+  <si>
+    <t>amaranth_bushel</t>
+  </si>
+  <si>
+    <t>sugar_cane</t>
+  </si>
+  <si>
+    <t>absorption</t>
+  </si>
+  <si>
+    <t>cactus</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>12x</t>
+  </si>
+  <si>
+    <t>8x</t>
+  </si>
+  <si>
+    <t>6x / 4x</t>
+  </si>
+  <si>
+    <t>potato, mermaids_gem, clover, snowball</t>
+  </si>
+  <si>
+    <t>oof</t>
+  </si>
+  <si>
+    <t>beetroot, clotted_cream</t>
+  </si>
+  <si>
+    <t>weakness</t>
+  </si>
+  <si>
+    <t>4x</t>
+  </si>
+  <si>
+    <t>glow_berries, moonstone_powder, stardust, paletur_fragments</t>
+  </si>
+  <si>
+    <t>invisibility</t>
+  </si>
+  <si>
+    <t>lightweight</t>
+  </si>
+  <si>
+    <t>golden_apple</t>
+  </si>
+  <si>
+    <t>enchanted_golden_apple</t>
   </si>
 </sst>
 </file>
@@ -137,7 +485,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,8 +533,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -331,13 +691,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -375,13 +855,78 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -392,6 +937,38 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}" name="Tabelle1" displayName="Tabelle1" ref="A20:I39" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A20:I39" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{01EC8C57-83BE-4610-A43F-E9C497C3103A}" name="Beverage Type" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{3AFBF746-223D-4849-8D15-6B5EBC41CD07}" name="Ferm.Mod" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{1E074399-223F-4717-8110-138418658072}" name="12">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{22C31000-51B9-4B7F-B422-644C6EF1B656}" name="24">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{8E06E958-7DE2-473E-B292-951C29C62EF1}" name="48">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{B74AAB8D-B30F-46F4-A6AE-682A6EAB9131}" name="72">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{C2DF63A0-3F23-448A-B439-244AD8443B28}" name="96">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{253E0318-1896-406A-A446-939D5EA3C3B1}" name="576">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{1D17B4C3-392F-435C-82A2-4BFC2C15EC49}" name="720" dataDxfId="2">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -691,15 +1268,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B33BBD-CB27-4534-9864-9F1639537D70}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="14" max="14" width="1.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -727,7 +1305,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="30">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
@@ -1057,51 +1635,51 @@
       </c>
       <c r="B14" s="36">
         <f>IF($B$4=0,0,LOG(B12*(0.5+B13/2)*(0.5+B9/2),1+$B$4)/100)</f>
-        <v>0.27526111294766215</v>
+        <v>4.5681297355864098E-2</v>
       </c>
       <c r="C14" s="20">
         <f t="shared" ref="C14:M14" si="2">IF($B$4=0,0,LOG(C12*(0.5+C13/2)*(0.5+C9/2),1+$B$4)/100)</f>
-        <v>0.3132789531169014</v>
+        <v>5.1990594891578673E-2</v>
       </c>
       <c r="D14" s="20">
         <f t="shared" si="2"/>
-        <v>0.33018871217533985</v>
+        <v>5.4796874803377964E-2</v>
       </c>
       <c r="E14" s="20">
         <f t="shared" si="2"/>
-        <v>0.34975167281535996</v>
+        <v>5.8043470054657584E-2</v>
       </c>
       <c r="F14" s="20">
         <f t="shared" si="2"/>
-        <v>0.31173383264612059</v>
+        <v>5.1734172518943015E-2</v>
       </c>
       <c r="G14" s="20">
         <f t="shared" si="2"/>
-        <v>0.27526111294766215</v>
+        <v>4.5681297355864098E-2</v>
       </c>
       <c r="H14" s="20">
         <f t="shared" si="2"/>
-        <v>0.27526111294766215</v>
+        <v>4.5681297355864098E-2</v>
       </c>
       <c r="I14" s="20">
         <f t="shared" si="2"/>
-        <v>0.27526111294766215</v>
+        <v>4.5681297355864098E-2</v>
       </c>
       <c r="J14" s="20">
         <f t="shared" si="2"/>
-        <v>0.27526111294766215</v>
+        <v>4.5681297355864098E-2</v>
       </c>
       <c r="K14" s="20">
         <f t="shared" si="2"/>
-        <v>0.27526111294766215</v>
+        <v>4.5681297355864098E-2</v>
       </c>
       <c r="L14" s="20">
         <f t="shared" si="2"/>
-        <v>0.27526111294766215</v>
+        <v>4.5681297355864098E-2</v>
       </c>
       <c r="M14" s="21">
         <f t="shared" si="2"/>
-        <v>0.27526111294766215</v>
+        <v>4.5681297355864098E-2</v>
       </c>
       <c r="O14" t="s">
         <v>13</v>
@@ -1163,7 +1741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1178,50 +1756,1313 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="45">
+        <v>1</v>
+      </c>
+      <c r="G18" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="45">
+        <v>0.4</v>
+      </c>
+      <c r="I18" s="44"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>39</v>
+      </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="K20" t="s">
+        <v>54</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="54">
+        <v>0</v>
+      </c>
+      <c r="C21" s="52">
+        <v>0</v>
+      </c>
+      <c r="D21" s="52">
+        <v>0</v>
+      </c>
+      <c r="E21" s="52">
+        <v>0</v>
+      </c>
+      <c r="F21" s="52">
+        <v>0</v>
+      </c>
+      <c r="G21" s="52">
+        <v>0</v>
+      </c>
+      <c r="H21" s="52">
+        <v>0</v>
+      </c>
+      <c r="I21" s="53">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3"/>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="55">
+        <v>1</v>
+      </c>
+      <c r="C22" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>3.0703893278913982E-2</v>
+      </c>
+      <c r="D22" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>4.0703893278913973E-2</v>
+      </c>
+      <c r="E22" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>5.0703893278913982E-2</v>
+      </c>
+      <c r="F22" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>5.6553518286125544E-2</v>
+      </c>
+      <c r="G22" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>6.0703893278913984E-2</v>
+      </c>
+      <c r="H22" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>8.6553518286125536E-2</v>
+      </c>
+      <c r="I22" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>8.9772799234999173E-2</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="55">
+        <v>1</v>
+      </c>
+      <c r="C23" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>3.0703893278913982E-2</v>
+      </c>
+      <c r="D23" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>4.0703893278913973E-2</v>
+      </c>
+      <c r="E23" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>5.0703893278913982E-2</v>
+      </c>
+      <c r="F23" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>5.6553518286125544E-2</v>
+      </c>
+      <c r="G23" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>6.0703893278913984E-2</v>
+      </c>
+      <c r="H23" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>8.6553518286125536E-2</v>
+      </c>
+      <c r="I23" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>8.9772799234999173E-2</v>
+      </c>
+      <c r="K23">
+        <v>12</v>
+      </c>
+      <c r="L23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="C24" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.11672957072511327</v>
+      </c>
+      <c r="D24" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.15474741089435257</v>
+      </c>
+      <c r="E24" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.19276525106359188</v>
+      </c>
+      <c r="F24" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.21500426192100733</v>
+      </c>
+      <c r="G24" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.23078309123283119</v>
+      </c>
+      <c r="H24" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.3290577824287253</v>
+      </c>
+      <c r="I24" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.34129679328614076</v>
+      </c>
+      <c r="K24">
+        <v>24</v>
+      </c>
+      <c r="L24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="C25" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.22329531957851728</v>
+      </c>
+      <c r="D25" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.2960207285519344</v>
+      </c>
+      <c r="E25" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.36874613752535157</v>
+      </c>
+      <c r="F25" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.41128777462441041</v>
+      </c>
+      <c r="G25" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.44147154649876869</v>
+      </c>
+      <c r="H25" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.62946400154466187</v>
+      </c>
+      <c r="I25" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.65287635390537835</v>
+      </c>
+      <c r="K25">
+        <v>24</v>
+      </c>
+      <c r="L25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <v/>
+      </c>
+      <c r="D26" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <v/>
+      </c>
+      <c r="E26" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <v/>
+      </c>
+      <c r="F26" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <v/>
+      </c>
+      <c r="G26" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <v/>
+      </c>
+      <c r="H26" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <v/>
+      </c>
+      <c r="I26" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="D27" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="E27" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="F27" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="G27" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="H27" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="I27" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="D28" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="E28" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="F28" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="G28" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="H28" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="I28" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="D29" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="E29" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="F29" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="G29" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="H29" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="I29" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="D30" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="E30" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="F30" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="G30" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="H30" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="I30" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="55">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C31" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.29427713455110671</v>
+      </c>
+      <c r="D31" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.3901207241173858</v>
+      </c>
+      <c r="E31" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.48596431368366494</v>
+      </c>
+      <c r="F31" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.54202921951444771</v>
+      </c>
+      <c r="G31" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.58180790324994403</v>
+      </c>
+      <c r="H31" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.82955998821328503</v>
+      </c>
+      <c r="I31" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.8604147324095236</v>
+      </c>
+      <c r="K31">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="55">
+        <v>0.05</v>
+      </c>
+      <c r="C32" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.4362009724867138</v>
+      </c>
+      <c r="D32" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.57826796331561836</v>
+      </c>
+      <c r="E32" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.72033495414452309</v>
+      </c>
+      <c r="F32" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.80343881636972869</v>
+      </c>
+      <c r="G32" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.86240194497342759</v>
+      </c>
+      <c r="H32" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>1.2296397888564425</v>
+      </c>
+      <c r="I32" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>1.275375144560372</v>
+      </c>
+      <c r="K32">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="C33" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.11672957072511327</v>
+      </c>
+      <c r="D33" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.15474741089435257</v>
+      </c>
+      <c r="E33" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.19276525106359188</v>
+      </c>
+      <c r="F33" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.21500426192100733</v>
+      </c>
+      <c r="G33" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.23078309123283119</v>
+      </c>
+      <c r="H33" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.3290577824287253</v>
+      </c>
+      <c r="I33" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.34129679328614076</v>
+      </c>
+      <c r="K33">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>5.2488652248753487E-2</v>
+      </c>
+      <c r="D34" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>6.9583765162268024E-2</v>
+      </c>
+      <c r="E34" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>8.6678878075782576E-2</v>
+      </c>
+      <c r="F34" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>9.6678878075782584E-2</v>
+      </c>
+      <c r="G34" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>0.10377399098929713</v>
+      </c>
+      <c r="H34" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>0.14796421681632624</v>
+      </c>
+      <c r="I34" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>0.15346761394845831</v>
+      </c>
+      <c r="K34">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="55">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C35" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.29427713455110671</v>
+      </c>
+      <c r="D35" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.3901207241173858</v>
+      </c>
+      <c r="E35" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.48596431368366494</v>
+      </c>
+      <c r="F35" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.54202921951444771</v>
+      </c>
+      <c r="G35" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.58180790324994403</v>
+      </c>
+      <c r="H35" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.82955998821328503</v>
+      </c>
+      <c r="I35" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.8604147324095236</v>
+      </c>
+      <c r="K35">
+        <v>24</v>
+      </c>
+      <c r="L35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="40">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>5.2488652248753487E-2</v>
+      </c>
+      <c r="D36" s="40">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>6.9583765162268024E-2</v>
+      </c>
+      <c r="E36" s="40">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>8.6678878075782576E-2</v>
+      </c>
+      <c r="F36" s="40">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>9.6678878075782584E-2</v>
+      </c>
+      <c r="G36" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>0.10377399098929713</v>
+      </c>
+      <c r="H36" s="40">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>0.14796421681632624</v>
+      </c>
+      <c r="I36" s="41">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>0.15346761394845831</v>
+      </c>
+      <c r="K36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v/>
+      </c>
+      <c r="D37" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v/>
+      </c>
+      <c r="E37" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v/>
+      </c>
+      <c r="F37" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v/>
+      </c>
+      <c r="G37" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v/>
+      </c>
+      <c r="H37" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v/>
+      </c>
+      <c r="I37" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <v/>
+      </c>
+      <c r="D38" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <v/>
+      </c>
+      <c r="E38" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <v/>
+      </c>
+      <c r="F38" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <v/>
+      </c>
+      <c r="G38" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <v/>
+      </c>
+      <c r="H38" s="40" t="str">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <v/>
+      </c>
+      <c r="I38" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="42"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="50" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="D39" s="50" t="str">
+        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="E39" s="50" t="str">
+        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="F39" s="50" t="str">
+        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="G39" s="50" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="H39" s="50" t="str">
+        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="I39" s="51" t="str">
+        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" t="s">
+        <v>84</v>
+      </c>
+      <c r="I43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" t="s">
+        <v>86</v>
+      </c>
+      <c r="F45" t="s">
+        <v>89</v>
+      </c>
+      <c r="I45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" t="s">
+        <v>86</v>
+      </c>
+      <c r="F46" t="s">
+        <v>89</v>
+      </c>
+      <c r="I46" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" t="s">
+        <v>89</v>
+      </c>
+      <c r="I47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E48" t="s">
+        <v>86</v>
+      </c>
+      <c r="F48" t="s">
+        <v>89</v>
+      </c>
+      <c r="I48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>43</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" t="s">
+        <v>99</v>
+      </c>
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+      <c r="I51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D52" t="s">
+        <v>86</v>
+      </c>
+      <c r="I52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" t="s">
+        <v>101</v>
+      </c>
+      <c r="I53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" t="s">
+        <v>86</v>
+      </c>
+      <c r="I56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" t="s">
+        <v>86</v>
+      </c>
+      <c r="E57" t="s">
+        <v>101</v>
+      </c>
+      <c r="I57" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" t="s">
+        <v>110</v>
+      </c>
+      <c r="I59" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>98</v>
+      </c>
+      <c r="I60" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" t="s">
+        <v>113</v>
+      </c>
+      <c r="D61" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" t="s">
+        <v>115</v>
+      </c>
+      <c r="I61" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" t="s">
+        <v>98</v>
+      </c>
+      <c r="C62" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" t="s">
+        <v>113</v>
+      </c>
+      <c r="E62" t="s">
+        <v>86</v>
+      </c>
+      <c r="I62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>73</v>
+      </c>
+      <c r="B63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" t="s">
+        <v>110</v>
+      </c>
+      <c r="E63" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" t="s">
+        <v>115</v>
+      </c>
+      <c r="G63" t="s">
+        <v>116</v>
+      </c>
+      <c r="I63" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>74</v>
+      </c>
+      <c r="B66" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" t="s">
+        <v>89</v>
+      </c>
+      <c r="I66" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="B67" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" t="s">
+        <v>86</v>
+      </c>
+      <c r="E67" t="s">
+        <v>87</v>
+      </c>
+      <c r="I67" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" t="s">
+        <v>87</v>
+      </c>
+      <c r="D68" t="s">
+        <v>113</v>
+      </c>
+      <c r="E68" t="s">
+        <v>86</v>
+      </c>
+      <c r="F68" t="s">
+        <v>89</v>
+      </c>
+      <c r="I68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" t="s">
+        <v>113</v>
+      </c>
+      <c r="E69" t="s">
+        <v>86</v>
+      </c>
+      <c r="F69" t="s">
+        <v>89</v>
+      </c>
+      <c r="I69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>78</v>
+      </c>
+      <c r="B70" t="s">
+        <v>98</v>
+      </c>
+      <c r="C70" t="s">
+        <v>100</v>
+      </c>
+      <c r="I70" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>80</v>
+      </c>
+      <c r="B72" t="s">
+        <v>91</v>
+      </c>
+      <c r="C72" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" t="s">
+        <v>89</v>
+      </c>
+      <c r="E72" t="s">
+        <v>130</v>
+      </c>
+      <c r="I72" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" t="s">
+        <v>91</v>
+      </c>
+      <c r="D75" t="s">
+        <v>92</v>
+      </c>
+      <c r="I75" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>82</v>
+      </c>
+      <c r="B76" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76" t="s">
+        <v>113</v>
+      </c>
+      <c r="E76" t="s">
+        <v>92</v>
+      </c>
+      <c r="I76" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77" t="s">
+        <v>133</v>
+      </c>
+      <c r="C77" t="s">
+        <v>134</v>
+      </c>
+      <c r="D77" t="s">
+        <v>111</v>
+      </c>
+      <c r="E77" t="s">
+        <v>87</v>
+      </c>
+      <c r="F77" t="s">
+        <v>86</v>
+      </c>
+      <c r="I77" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:M13">
@@ -1262,5 +3103,8 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adjusted beverage ingredients / outputs
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D85C27-8480-4A0D-8587-B88785C631A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59129C6-B48B-491F-ADF7-00ED5F027B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34395" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
+    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="140">
   <si>
     <t>thickness</t>
   </si>
@@ -383,9 +383,6 @@
     <t>poison</t>
   </si>
   <si>
-    <t>unluck</t>
-  </si>
-  <si>
     <t>blazing</t>
   </si>
   <si>
@@ -428,9 +425,6 @@
     <t>weakness</t>
   </si>
   <si>
-    <t>4x</t>
-  </si>
-  <si>
     <t>glow_berries, moonstone_powder, stardust, paletur_fragments</t>
   </si>
   <si>
@@ -444,6 +438,21 @@
   </si>
   <si>
     <t>enchanted_golden_apple</t>
+  </si>
+  <si>
+    <t>apple_liquor</t>
+  </si>
+  <si>
+    <t>apples, sugar</t>
+  </si>
+  <si>
+    <t>millenia_disease</t>
+  </si>
+  <si>
+    <t>vulnerability</t>
+  </si>
+  <si>
+    <t>stiffness</t>
   </si>
 </sst>
 </file>
@@ -1271,13 +1280,13 @@
   <dimension ref="A1:O77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K56" sqref="K56"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.125" customWidth="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="2" max="13" width="12.5" customWidth="1"/>
     <col min="14" max="14" width="1.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2545,26 +2554,72 @@
         <v/>
       </c>
     </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" t="s">
+        <v>84</v>
+      </c>
+      <c r="I42" t="s">
+        <v>97</v>
+      </c>
+    </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
         <v>90</v>
       </c>
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
       <c r="D43" t="s">
         <v>84</v>
       </c>
+      <c r="F43" t="s">
+        <v>86</v>
+      </c>
+      <c r="G43" t="s">
+        <v>139</v>
+      </c>
       <c r="I43" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" t="s">
+        <v>86</v>
+      </c>
+      <c r="G44" t="s">
+        <v>139</v>
+      </c>
+      <c r="I44" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
         <v>85</v>
@@ -2572,22 +2627,22 @@
       <c r="D45" t="s">
         <v>84</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>86</v>
       </c>
-      <c r="F45" t="s">
-        <v>89</v>
+      <c r="G45" t="s">
+        <v>139</v>
       </c>
       <c r="I45" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
         <v>85</v>
@@ -2595,160 +2650,131 @@
       <c r="D46" t="s">
         <v>84</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>86</v>
       </c>
-      <c r="F46" t="s">
-        <v>89</v>
+      <c r="G46" t="s">
+        <v>139</v>
       </c>
       <c r="I46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" t="s">
-        <v>85</v>
-      </c>
-      <c r="D47" t="s">
-        <v>84</v>
-      </c>
-      <c r="E47" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" t="s">
         <v>86</v>
       </c>
-      <c r="F47" t="s">
-        <v>89</v>
-      </c>
-      <c r="I47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" t="s">
-        <v>85</v>
-      </c>
-      <c r="D48" t="s">
-        <v>84</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="I49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" t="s">
+        <v>99</v>
+      </c>
+      <c r="F50" t="s">
         <v>86</v>
       </c>
-      <c r="F48" t="s">
-        <v>89</v>
-      </c>
-      <c r="I48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I50" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
         <v>99</v>
       </c>
       <c r="D51" t="s">
+        <v>101</v>
+      </c>
+      <c r="F51" t="s">
         <v>86</v>
       </c>
       <c r="I51" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54" t="s">
+        <v>86</v>
+      </c>
+      <c r="I54" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
         <v>88</v>
       </c>
-      <c r="C52" t="s">
-        <v>91</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="F55" t="s">
         <v>86</v>
       </c>
-      <c r="I52" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>65</v>
-      </c>
-      <c r="B53" t="s">
-        <v>100</v>
-      </c>
-      <c r="C53" t="s">
-        <v>99</v>
-      </c>
-      <c r="D53" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" t="s">
-        <v>101</v>
-      </c>
-      <c r="I53" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I55" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B56" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s">
         <v>98</v>
       </c>
       <c r="D56" t="s">
+        <v>101</v>
+      </c>
+      <c r="F56" t="s">
         <v>86</v>
       </c>
       <c r="I56" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" t="s">
-        <v>98</v>
-      </c>
-      <c r="D57" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" t="s">
-        <v>101</v>
-      </c>
-      <c r="I57" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2760,13 +2786,16 @@
         <v>84</v>
       </c>
       <c r="C58" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" t="s">
         <v>85</v>
       </c>
-      <c r="D58" t="s">
-        <v>86</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>87</v>
+      </c>
+      <c r="G58" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -2774,16 +2803,19 @@
         <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C59" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D59" t="s">
-        <v>109</v>
-      </c>
-      <c r="E59" t="s">
         <v>110</v>
+      </c>
+      <c r="F59" t="s">
+        <v>87</v>
+      </c>
+      <c r="G59" t="s">
+        <v>89</v>
       </c>
       <c r="I59" t="s">
         <v>107</v>
@@ -2799,79 +2831,91 @@
       <c r="C60" t="s">
         <v>98</v>
       </c>
+      <c r="D60" t="s">
+        <v>132</v>
+      </c>
+      <c r="F60" t="s">
+        <v>87</v>
+      </c>
+      <c r="G60" t="s">
+        <v>89</v>
+      </c>
       <c r="I60" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="C61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" t="s">
         <v>113</v>
       </c>
-      <c r="D61" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" t="s">
-        <v>115</v>
+      <c r="F61" t="s">
+        <v>87</v>
+      </c>
+      <c r="G61" t="s">
+        <v>89</v>
       </c>
       <c r="I61" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B62" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" t="s">
         <v>98</v>
       </c>
-      <c r="C62" t="s">
-        <v>99</v>
-      </c>
       <c r="D62" t="s">
-        <v>113</v>
-      </c>
-      <c r="E62" t="s">
-        <v>86</v>
+        <v>110</v>
+      </c>
+      <c r="F62" t="s">
+        <v>87</v>
+      </c>
+      <c r="G62" t="s">
+        <v>89</v>
       </c>
       <c r="I62" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B63" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>110</v>
-      </c>
-      <c r="E63" t="s">
+        <v>88</v>
+      </c>
+      <c r="F63" t="s">
         <v>87</v>
       </c>
-      <c r="F63" t="s">
-        <v>115</v>
-      </c>
       <c r="G63" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="I63" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -2882,126 +2926,142 @@
         <v>110</v>
       </c>
       <c r="C66" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="D66" t="s">
-        <v>89</v>
+        <v>113</v>
+      </c>
+      <c r="F66" t="s">
+        <v>129</v>
+      </c>
+      <c r="G66" t="s">
+        <v>115</v>
       </c>
       <c r="I66" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B67" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C67" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="D67" t="s">
-        <v>86</v>
-      </c>
-      <c r="E67" t="s">
-        <v>87</v>
+        <v>113</v>
+      </c>
+      <c r="F67" t="s">
+        <v>129</v>
+      </c>
+      <c r="G67" t="s">
+        <v>115</v>
       </c>
       <c r="I67" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
+        <v>98</v>
+      </c>
+      <c r="C68" t="s">
         <v>100</v>
-      </c>
-      <c r="C68" t="s">
-        <v>87</v>
       </c>
       <c r="D68" t="s">
         <v>113</v>
       </c>
-      <c r="E68" t="s">
-        <v>86</v>
-      </c>
       <c r="F68" t="s">
-        <v>89</v>
+        <v>129</v>
+      </c>
+      <c r="G68" t="s">
+        <v>115</v>
       </c>
       <c r="I68" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D69" t="s">
         <v>113</v>
       </c>
-      <c r="E69" t="s">
-        <v>86</v>
-      </c>
       <c r="F69" t="s">
-        <v>89</v>
+        <v>129</v>
+      </c>
+      <c r="G69" t="s">
+        <v>115</v>
       </c>
       <c r="I69" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B70" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="C70" t="s">
-        <v>100</v>
+        <v>113</v>
+      </c>
+      <c r="D70" t="s">
+        <v>92</v>
+      </c>
+      <c r="F70" t="s">
+        <v>129</v>
+      </c>
+      <c r="G70" t="s">
+        <v>115</v>
       </c>
       <c r="I70" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>128</v>
+        <v>100</v>
+      </c>
+      <c r="C71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D71" t="s">
+        <v>92</v>
+      </c>
+      <c r="F71" t="s">
+        <v>129</v>
+      </c>
+      <c r="G71" t="s">
+        <v>115</v>
+      </c>
+      <c r="I71" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B72" t="s">
-        <v>91</v>
-      </c>
-      <c r="C72" t="s">
-        <v>100</v>
-      </c>
-      <c r="D72" t="s">
-        <v>89</v>
-      </c>
-      <c r="E72" t="s">
-        <v>130</v>
-      </c>
-      <c r="I72" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I74" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3009,7 +3069,7 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" t="s">
         <v>91</v>
@@ -3018,7 +3078,7 @@
         <v>92</v>
       </c>
       <c r="I75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3026,7 +3086,7 @@
         <v>82</v>
       </c>
       <c r="B76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C76" t="s">
         <v>91</v>
@@ -3038,7 +3098,7 @@
         <v>92</v>
       </c>
       <c r="I76" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -3046,22 +3106,22 @@
         <v>83</v>
       </c>
       <c r="B77" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C77" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D77" t="s">
         <v>111</v>
       </c>
-      <c r="E77" t="s">
-        <v>87</v>
-      </c>
       <c r="F77" t="s">
-        <v>86</v>
+        <v>138</v>
+      </c>
+      <c r="G77" t="s">
+        <v>137</v>
       </c>
       <c r="I77" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished beverage calculations & effects
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59129C6-B48B-491F-ADF7-00ED5F027B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0459D5-76B9-4BF6-87AD-C93BC3E8E319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="146">
   <si>
     <t>thickness</t>
   </si>
@@ -131,30 +131,9 @@
     <t>3 days</t>
   </si>
   <si>
-    <t>1 month</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
     <t>72</t>
   </si>
   <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>576</t>
-  </si>
-  <si>
-    <t>720</t>
-  </si>
-  <si>
     <t>beer, ale, lager, porter</t>
   </si>
   <si>
@@ -173,9 +152,6 @@
     <t>Liquor / Creme Liquor</t>
   </si>
   <si>
-    <t>gin, rum, tequilla, vodka, mint_schnapps, rabbit_poison, damassine</t>
-  </si>
-  <si>
     <t>Golden Apple Cider</t>
   </si>
   <si>
@@ -453,6 +429,48 @@
   </si>
   <si>
     <t>stiffness</t>
+  </si>
+  <si>
+    <t>wheat, clotted_cream, egg</t>
+  </si>
+  <si>
+    <t>high thickness</t>
+  </si>
+  <si>
+    <t>high %</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>gin, rum, tequilla, vodka, mint_schnapps, damassine</t>
+  </si>
+  <si>
+    <t>Rabbit Poison</t>
+  </si>
+  <si>
+    <t>1 RL day = 72 MC days</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>288</t>
+  </si>
+  <si>
+    <t>1008</t>
+  </si>
+  <si>
+    <t>2160</t>
+  </si>
+  <si>
+    <t>30 days</t>
   </si>
 </sst>
 </file>
@@ -462,7 +480,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,6 +506,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -826,7 +851,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -884,6 +909,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -891,6 +918,18 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -909,18 +948,6 @@
           <color indexed="64"/>
         </left>
         <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
         <top/>
         <bottom/>
         <vertical/>
@@ -952,28 +979,28 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}" name="Tabelle1" displayName="Tabelle1" ref="A20:I39" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A20:I39" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{01EC8C57-83BE-4610-A43F-E9C497C3103A}" name="Beverage Type" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{3AFBF746-223D-4849-8D15-6B5EBC41CD07}" name="Ferm.Mod" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{1E074399-223F-4717-8110-138418658072}" name="12">
+    <tableColumn id="1" xr3:uid="{01EC8C57-83BE-4610-A43F-E9C497C3103A}" name="Beverage Type" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{3AFBF746-223D-4849-8D15-6B5EBC41CD07}" name="Ferm.Mod" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{1E074399-223F-4717-8110-138418658072}" name="32">
       <calculatedColumnFormula>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{22C31000-51B9-4B7F-B422-644C6EF1B656}" name="24">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{22C31000-51B9-4B7F-B422-644C6EF1B656}" name="72">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{8E06E958-7DE2-473E-B292-951C29C62EF1}" name="48">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{8E06E958-7DE2-473E-B292-951C29C62EF1}" name="144">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B74AAB8D-B30F-46F4-A6AE-682A6EAB9131}" name="72">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{B74AAB8D-B30F-46F4-A6AE-682A6EAB9131}" name="216">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C2DF63A0-3F23-448A-B439-244AD8443B28}" name="96">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{C2DF63A0-3F23-448A-B439-244AD8443B28}" name="288">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{253E0318-1896-406A-A446-939D5EA3C3B1}" name="576">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{253E0318-1896-406A-A446-939D5EA3C3B1}" name="1008">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1D17B4C3-392F-435C-82A2-4BFC2C15EC49}" name="720" dataDxfId="2">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+    <tableColumn id="9" xr3:uid="{1D17B4C3-392F-435C-82A2-4BFC2C15EC49}" name="2160" dataDxfId="0">
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1277,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B33BBD-CB27-4534-9864-9F1639537D70}">
-  <dimension ref="A1:O77"/>
+  <dimension ref="A1:Y77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1761,13 +1788,15 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="K17" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B18" s="43"/>
       <c r="C18" s="43"/>
@@ -1812,7 +1841,7 @@
         <v>25</v>
       </c>
       <c r="I19" s="48" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1824,41 +1853,41 @@
         <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>36</v>
+        <v>139</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>37</v>
+        <v>142</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>38</v>
+        <v>143</v>
       </c>
       <c r="I20" s="38" t="s">
-        <v>39</v>
+        <v>144</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="37" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B21" s="54">
         <v>0</v>
@@ -1889,7 +1918,7 @@
         <v>4</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="M21" s="3"/>
     </row>
@@ -1898,125 +1927,125 @@
         <v>21</v>
       </c>
       <c r="B22" s="55">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C22" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>3.0703893278913982E-2</v>
+        <v>3.833943903789129E-2</v>
       </c>
       <c r="D22" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>4.0703893278913973E-2</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>4.8339439037891292E-2</v>
       </c>
       <c r="E22" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>5.0703893278913982E-2</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>5.6886995494648568E-2</v>
       </c>
       <c r="F22" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>5.6553518286125544E-2</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>6.1886995494648572E-2</v>
       </c>
       <c r="G22" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>6.0703893278913984E-2</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>6.543455195140585E-2</v>
       </c>
       <c r="H22" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>8.6553518286125536E-2</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>8.0883020185091359E-2</v>
       </c>
       <c r="I22" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>8.9772799234999173E-2</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
+        <v>9.028136343098643E-2</v>
       </c>
       <c r="K22">
         <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B23" s="55">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="C23" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
-        <v>3.0703893278913982E-2</v>
+        <v>3.833943903789129E-2</v>
       </c>
       <c r="D23" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
-        <v>4.0703893278913973E-2</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>4.8339439037891292E-2</v>
       </c>
       <c r="E23" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
-        <v>5.0703893278913982E-2</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>5.6886995494648568E-2</v>
       </c>
       <c r="F23" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
-        <v>5.6553518286125544E-2</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>6.1886995494648572E-2</v>
       </c>
       <c r="G23" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
-        <v>6.0703893278913984E-2</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>6.543455195140585E-2</v>
       </c>
       <c r="H23" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
-        <v>8.6553518286125536E-2</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>8.0883020185091359E-2</v>
       </c>
       <c r="I23" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
-        <v>8.9772799234999173E-2</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+        <v>9.028136343098643E-2</v>
       </c>
       <c r="K23">
         <v>12</v>
       </c>
       <c r="L23" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B24" s="55">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C24" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.11672957072511327</v>
+        <v>0.13933008328271637</v>
       </c>
       <c r="D24" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.15474741089435257</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.17567127313294212</v>
       </c>
       <c r="E24" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.19276525106359188</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.20673411032799602</v>
       </c>
       <c r="F24" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.21500426192100733</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.22490470525310891</v>
       </c>
       <c r="G24" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.23078309123283119</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.23779694752304992</v>
       </c>
       <c r="H24" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.3290577824287253</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.2939385192206046</v>
       </c>
       <c r="I24" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.34129679328614076</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
+        <v>0.32809321683827058</v>
       </c>
       <c r="K24">
         <v>24</v>
       </c>
       <c r="L24" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -2024,41 +2053,41 @@
         <v>22</v>
       </c>
       <c r="B25" s="55">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
       <c r="C25" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.22329531957851728</v>
+        <v>0.26396508983953099</v>
       </c>
       <c r="D25" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.2960207285519344</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.33281458176314815</v>
       </c>
       <c r="E25" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.36874613752535157</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.39166407368676537</v>
       </c>
       <c r="F25" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.41128777462441041</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.42608881964857398</v>
       </c>
       <c r="G25" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.44147154649876869</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.45051356561038253</v>
       </c>
       <c r="H25" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.62946400154466187</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.55687548449912128</v>
       </c>
       <c r="I25" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.65287635390537835</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
+        <v>0.62158260023948475</v>
       </c>
       <c r="K25">
         <v>24</v>
       </c>
       <c r="L25" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -2069,27 +2098,27 @@
         <v/>
       </c>
       <c r="D26" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
       <c r="E26" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
       <c r="F26" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
       <c r="G26" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
       <c r="H26" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
       <c r="I26" s="41" t="str">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
     </row>
@@ -2101,27 +2130,27 @@
         <v/>
       </c>
       <c r="D27" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
       <c r="E27" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
       <c r="F27" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
       <c r="G27" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
       <c r="H27" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
       <c r="I27" s="41" t="str">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
     </row>
@@ -2133,27 +2162,27 @@
         <v/>
       </c>
       <c r="D28" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
       <c r="E28" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
       <c r="F28" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
       <c r="G28" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
       <c r="H28" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
       <c r="I28" s="41" t="str">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
     </row>
@@ -2165,27 +2194,27 @@
         <v/>
       </c>
       <c r="D29" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
       <c r="E29" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
       <c r="F29" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
       <c r="G29" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
       <c r="H29" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
       <c r="I29" s="41" t="str">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
     </row>
@@ -2197,64 +2226,64 @@
         <v/>
       </c>
       <c r="D30" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
       <c r="E30" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
       <c r="F30" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
       <c r="G30" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
       <c r="H30" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
       <c r="I30" s="41" t="str">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B31" s="55">
-        <v>7.4999999999999997E-2</v>
+        <v>0.1</v>
       </c>
       <c r="C31" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.29427713455110671</v>
+        <v>0.32620450042629268</v>
       </c>
       <c r="D31" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.3901207241173858</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.41128777462441041</v>
       </c>
       <c r="E31" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.48596431368366494</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.48401318359782758</v>
       </c>
       <c r="F31" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.54202921951444771</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.52655482069688653</v>
       </c>
       <c r="G31" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.58180790324994403</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.55673859257124469</v>
       </c>
       <c r="H31" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.82955998821328503</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.68817921843800245</v>
       </c>
       <c r="I31" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.8604147324095236</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
+        <v>0.76814339997785419</v>
       </c>
       <c r="K31">
         <v>48</v>
@@ -2262,235 +2291,239 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B32" s="55">
-        <v>0.05</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="C32" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.4362009724867138</v>
+        <v>0.42989940785288216</v>
       </c>
       <c r="D32" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.57826796331561836</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.54202921951444771</v>
       </c>
       <c r="E32" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.72033495414452309</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.63787280908072685</v>
       </c>
       <c r="F32" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.80343881636972869</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.69393771491150957</v>
       </c>
       <c r="G32" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.86240194497342759</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.733716398647006</v>
       </c>
       <c r="H32" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>1.2296397888564425</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>0.90693978199728931</v>
       </c>
       <c r="I32" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>1.275375144560372</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
+        <v>1.0123232278065855</v>
       </c>
       <c r="K32">
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B33" s="55">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C33" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.11672957072511327</v>
+        <v>0.13933008328271637</v>
       </c>
       <c r="D33" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.15474741089435257</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.17567127313294212</v>
       </c>
       <c r="E33" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.19276525106359188</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.20673411032799602</v>
       </c>
       <c r="F33" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.21500426192100733</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.22490470525310891</v>
       </c>
       <c r="G33" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.23078309123283119</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.23779694752304992</v>
       </c>
       <c r="H33" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.3290577824287253</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.2939385192206046</v>
       </c>
       <c r="I33" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.34129679328614076</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
+        <v>0.32809321683827058</v>
       </c>
       <c r="K33">
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B34" s="55">
         <v>0.5</v>
       </c>
       <c r="C34" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>5.2488652248753487E-2</v>
+        <v>7.6678878075782581E-2</v>
       </c>
       <c r="D34" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>6.9583765162268024E-2</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>9.6678878075782584E-2</v>
       </c>
       <c r="E34" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>8.6678878075782576E-2</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>0.11377399098929714</v>
       </c>
       <c r="F34" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>9.6678878075782584E-2</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>0.12377399098929714</v>
       </c>
       <c r="G34" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>0.10377399098929713</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>0.1308691039028117</v>
       </c>
       <c r="H34" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>0.14796421681632624</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>0.16176604037018272</v>
       </c>
       <c r="I34" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>0.15346761394845831</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
+        <v>0.18056272686197286</v>
       </c>
       <c r="K34">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B35" s="55">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C35" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.29427713455110671</v>
+        <v>0.42989940785288216</v>
       </c>
       <c r="D35" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.3901207241173858</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.54202921951444771</v>
       </c>
       <c r="E35" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.48596431368366494</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.63787280908072685</v>
       </c>
       <c r="F35" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.54202921951444771</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.69393771491150957</v>
       </c>
       <c r="G35" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.58180790324994403</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.733716398647006</v>
       </c>
       <c r="H35" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.82955998821328503</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>0.90693978199728931</v>
       </c>
       <c r="I35" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.8604147324095236</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
+        <v>1.0123232278065855</v>
       </c>
       <c r="K35">
         <v>24</v>
       </c>
       <c r="L35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B36" s="55">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C36" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>5.2488652248753487E-2</v>
+        <v>4.485426827170242E-2</v>
       </c>
       <c r="D36" s="40">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>6.9583765162268024E-2</v>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>5.6553518286125544E-2</v>
       </c>
       <c r="E36" s="40">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>8.6678878075782576E-2</v>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>6.6553518286125546E-2</v>
       </c>
       <c r="F36" s="40">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>9.6678878075782584E-2</v>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>7.2403143293337108E-2</v>
       </c>
       <c r="G36" s="40">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>0.10377399098929713</v>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>7.6553518286125541E-2</v>
       </c>
       <c r="H36" s="40">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>0.14796421681632624</v>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>9.4627067506701593E-2</v>
       </c>
       <c r="I36" s="41">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>0.15346761394845831</v>
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
+        <v>0.10562242424221072</v>
       </c>
       <c r="K36">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="40" t="str">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="55">
+        <v>1</v>
+      </c>
+      <c r="C37" s="40">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
-        <v/>
-      </c>
-      <c r="D37" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
-        <v/>
-      </c>
-      <c r="E37" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
-        <v/>
-      </c>
-      <c r="F37" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
-        <v/>
-      </c>
-      <c r="G37" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
-        <v/>
-      </c>
-      <c r="H37" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
-        <v/>
-      </c>
-      <c r="I37" s="41" t="str">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>4.485426827170242E-2</v>
+      </c>
+      <c r="D37" s="40">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v>5.6553518286125544E-2</v>
+      </c>
+      <c r="E37" s="40">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v>6.6553518286125546E-2</v>
+      </c>
+      <c r="F37" s="40">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="G37" s="40">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v>7.6553518286125541E-2</v>
+      </c>
+      <c r="H37" s="40">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v>9.4627067506701593E-2</v>
+      </c>
+      <c r="I37" s="41">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+        <v>0.10562242424221072</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="55"/>
       <c r="C38" s="40" t="str">
@@ -2498,31 +2531,31 @@
         <v/>
       </c>
       <c r="D38" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
       <c r="E38" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
       <c r="F38" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
       <c r="G38" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
       <c r="H38" s="40" t="str">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
       <c r="I38" s="41" t="str">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="42"/>
       <c r="B39" s="56"/>
       <c r="C39" s="50" t="str">
@@ -2530,598 +2563,746 @@
         <v/>
       </c>
       <c r="D39" s="50" t="str">
-        <f>IF(Tabelle1[[#This Row],[12]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
       <c r="E39" s="50" t="str">
-        <f>IF(Tabelle1[[#This Row],[24]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
       <c r="F39" s="50" t="str">
-        <f>IF(Tabelle1[[#This Row],[48]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
       <c r="G39" s="50" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
       <c r="H39" s="50" t="str">
-        <f>IF(Tabelle1[[#This Row],[96]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
       <c r="I39" s="51" t="str">
-        <f>IF(Tabelle1[[#This Row],[576]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="I42" t="s">
+        <v>89</v>
+      </c>
+      <c r="S42" s="58"/>
+      <c r="T42" s="58"/>
+      <c r="U42" s="58"/>
+      <c r="V42" s="58"/>
+      <c r="W42" s="58"/>
+      <c r="X42" s="58"/>
+      <c r="Y42" s="58"/>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43" t="s">
+        <v>78</v>
+      </c>
+      <c r="I43" t="s">
+        <v>86</v>
+      </c>
+      <c r="S43" s="58"/>
+      <c r="T43" s="58"/>
+      <c r="U43" s="58"/>
+      <c r="V43" s="58"/>
+      <c r="W43" s="58"/>
+      <c r="X43" s="58"/>
+      <c r="Y43" s="58"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" t="s">
+        <v>131</v>
+      </c>
+      <c r="G44" t="s">
+        <v>78</v>
+      </c>
+      <c r="I44" t="s">
+        <v>85</v>
+      </c>
+      <c r="S44" s="58"/>
+      <c r="T44" s="58"/>
+      <c r="U44" s="58"/>
+      <c r="V44" s="58"/>
+      <c r="W44" s="58"/>
+      <c r="X44" s="58"/>
+      <c r="Y44" s="58"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" t="s">
+        <v>131</v>
+      </c>
+      <c r="G45" t="s">
+        <v>78</v>
+      </c>
+      <c r="I45" t="s">
+        <v>87</v>
+      </c>
+      <c r="S45" s="58"/>
+      <c r="T45" s="58"/>
+      <c r="U45" s="58"/>
+      <c r="V45" s="58"/>
+      <c r="W45" s="58"/>
+      <c r="X45" s="58"/>
+      <c r="Y45" s="58"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" t="s">
+        <v>78</v>
+      </c>
+      <c r="I46" t="s">
+        <v>88</v>
+      </c>
+      <c r="S46" s="58"/>
+      <c r="T46" s="58"/>
+      <c r="U46" s="58"/>
+      <c r="V46" s="58"/>
+      <c r="W46" s="58"/>
+      <c r="X46" s="58"/>
+      <c r="Y46" s="58"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="S47" s="58"/>
+      <c r="T47" s="58"/>
+      <c r="U47" s="58"/>
+      <c r="V47" s="58"/>
+      <c r="W47" s="58"/>
+      <c r="X47" s="58"/>
+      <c r="Y47" s="58"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>116</v>
+      </c>
+      <c r="S48" s="58"/>
+      <c r="T48" s="58"/>
+      <c r="U48" s="58"/>
+      <c r="V48" s="58"/>
+      <c r="W48" s="58"/>
+      <c r="X48" s="58"/>
+      <c r="Y48" s="58"/>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
         <v>90</v>
       </c>
-      <c r="D42" t="s">
-        <v>84</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="C49" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" t="s">
+        <v>78</v>
+      </c>
+      <c r="I49" t="s">
+        <v>94</v>
+      </c>
+      <c r="S49" s="58"/>
+      <c r="T49" s="58"/>
+      <c r="U49" s="58"/>
+      <c r="V49" s="58"/>
+      <c r="W49" s="58"/>
+      <c r="X49" s="58"/>
+      <c r="Y49" s="58"/>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" t="s">
+        <v>91</v>
+      </c>
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+      <c r="G50" t="s">
+        <v>78</v>
+      </c>
+      <c r="I50" t="s">
+        <v>95</v>
+      </c>
+      <c r="S50" s="58"/>
+      <c r="T50" s="58"/>
+      <c r="U50" s="58"/>
+      <c r="V50" s="58"/>
+      <c r="W50" s="58"/>
+      <c r="X50" s="58"/>
+      <c r="Y50" s="58"/>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" t="s">
+        <v>121</v>
+      </c>
+      <c r="G51" t="s">
+        <v>78</v>
+      </c>
+      <c r="I51" t="s">
+        <v>96</v>
+      </c>
+      <c r="S51" s="58"/>
+      <c r="T51" s="58"/>
+      <c r="U51" s="58"/>
+      <c r="V51" s="58"/>
+      <c r="W51" s="58"/>
+      <c r="X51" s="58"/>
+      <c r="Y51" s="58"/>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="S52" s="58"/>
+      <c r="T52" s="58"/>
+      <c r="U52" s="58"/>
+      <c r="V52" s="58"/>
+      <c r="W52" s="58"/>
+      <c r="X52" s="58"/>
+      <c r="Y52" s="58"/>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>117</v>
+      </c>
+      <c r="S53" s="58"/>
+      <c r="T53" s="58"/>
+      <c r="U53" s="58"/>
+      <c r="V53" s="58"/>
+      <c r="W53" s="58"/>
+      <c r="X53" s="58"/>
+      <c r="Y53" s="58"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>127</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" t="s">
+        <v>90</v>
+      </c>
+      <c r="F54" t="s">
+        <v>79</v>
+      </c>
+      <c r="G54" t="s">
+        <v>78</v>
+      </c>
+      <c r="I54" t="s">
+        <v>128</v>
+      </c>
+      <c r="S54" s="58"/>
+      <c r="T54" s="58"/>
+      <c r="U54" s="58"/>
+      <c r="V54" s="58"/>
+      <c r="W54" s="58"/>
+      <c r="X54" s="58"/>
+      <c r="Y54" s="58"/>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>90</v>
+      </c>
+      <c r="F55" t="s">
+        <v>79</v>
+      </c>
+      <c r="G55" t="s">
+        <v>78</v>
+      </c>
+      <c r="I55" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="S55" s="58"/>
+      <c r="T55" s="58"/>
+      <c r="U55" s="58"/>
+      <c r="V55" s="58"/>
+      <c r="W55" s="58"/>
+      <c r="X55" s="58"/>
+      <c r="Y55" s="58"/>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D56" t="s">
+        <v>93</v>
+      </c>
+      <c r="F56" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" t="s">
+        <v>78</v>
+      </c>
+      <c r="I56" t="s">
+        <v>98</v>
+      </c>
+      <c r="S56" s="58"/>
+      <c r="T56" s="58"/>
+      <c r="U56" s="58"/>
+      <c r="V56" s="58"/>
+      <c r="W56" s="58"/>
+      <c r="X56" s="58"/>
+      <c r="Y56" s="58"/>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="S57" s="58"/>
+      <c r="T57" s="58"/>
+      <c r="U57" s="58"/>
+      <c r="V57" s="58"/>
+      <c r="W57" s="58"/>
+      <c r="X57" s="58"/>
+      <c r="Y57" s="58"/>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>60</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B58" t="s">
+        <v>76</v>
+      </c>
+      <c r="C58" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" t="s">
+        <v>105</v>
+      </c>
+      <c r="F58" t="s">
+        <v>79</v>
+      </c>
+      <c r="G58" t="s">
+        <v>81</v>
+      </c>
+      <c r="I58" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" t="s">
         <v>90</v>
       </c>
-      <c r="C43" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" t="s">
-        <v>84</v>
-      </c>
-      <c r="F43" t="s">
-        <v>86</v>
-      </c>
-      <c r="G43" t="s">
-        <v>139</v>
-      </c>
-      <c r="I43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" t="s">
-        <v>86</v>
-      </c>
-      <c r="G44" t="s">
-        <v>139</v>
-      </c>
-      <c r="I44" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="D59" t="s">
+        <v>102</v>
+      </c>
+      <c r="F59" t="s">
+        <v>79</v>
+      </c>
+      <c r="G59" t="s">
+        <v>81</v>
+      </c>
+      <c r="I59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>62</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" t="s">
+        <v>124</v>
+      </c>
+      <c r="F60" t="s">
+        <v>79</v>
+      </c>
+      <c r="G60" t="s">
+        <v>81</v>
+      </c>
+      <c r="I60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61" t="s">
         <v>91</v>
       </c>
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" t="s">
-        <v>84</v>
-      </c>
-      <c r="F45" t="s">
-        <v>86</v>
-      </c>
-      <c r="G45" t="s">
-        <v>139</v>
-      </c>
-      <c r="I45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="F61" t="s">
+        <v>79</v>
+      </c>
+      <c r="G61" t="s">
+        <v>81</v>
+      </c>
+      <c r="I61" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62" t="s">
+        <v>83</v>
+      </c>
+      <c r="C62" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62" t="s">
+        <v>102</v>
+      </c>
+      <c r="F62" t="s">
+        <v>79</v>
+      </c>
+      <c r="G62" t="s">
+        <v>81</v>
+      </c>
+      <c r="I62" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>63</v>
       </c>
-      <c r="B46" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" t="s">
-        <v>85</v>
-      </c>
-      <c r="D46" t="s">
-        <v>84</v>
-      </c>
-      <c r="F46" t="s">
-        <v>86</v>
-      </c>
-      <c r="G46" t="s">
-        <v>139</v>
-      </c>
-      <c r="I46" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="I48" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" t="s">
-        <v>86</v>
-      </c>
-      <c r="I49" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" t="s">
-        <v>99</v>
-      </c>
-      <c r="F50" t="s">
-        <v>86</v>
-      </c>
-      <c r="I50" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>65</v>
-      </c>
-      <c r="B51" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" t="s">
-        <v>101</v>
-      </c>
-      <c r="F51" t="s">
-        <v>86</v>
-      </c>
-      <c r="I51" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I53" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="B63" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" t="s">
+        <v>105</v>
+      </c>
+      <c r="D63" t="s">
+        <v>80</v>
+      </c>
+      <c r="F63" t="s">
+        <v>79</v>
+      </c>
+      <c r="G63" t="s">
+        <v>81</v>
+      </c>
+      <c r="I63" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B65" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="B54" t="s">
-        <v>98</v>
-      </c>
-      <c r="C54" t="s">
-        <v>98</v>
-      </c>
-      <c r="F54" t="s">
-        <v>86</v>
-      </c>
-      <c r="I54" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>66</v>
-      </c>
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" t="s">
-        <v>98</v>
-      </c>
-      <c r="F55" t="s">
-        <v>86</v>
-      </c>
-      <c r="I55" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>67</v>
-      </c>
-      <c r="B56" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" t="s">
-        <v>98</v>
-      </c>
-      <c r="D56" t="s">
-        <v>101</v>
-      </c>
-      <c r="F56" t="s">
-        <v>86</v>
-      </c>
-      <c r="I56" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" t="s">
-        <v>84</v>
-      </c>
-      <c r="C58" t="s">
-        <v>98</v>
-      </c>
-      <c r="D58" t="s">
-        <v>85</v>
-      </c>
-      <c r="F58" t="s">
-        <v>87</v>
-      </c>
-      <c r="G58" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>69</v>
-      </c>
-      <c r="B59" t="s">
-        <v>109</v>
-      </c>
-      <c r="C59" t="s">
-        <v>98</v>
-      </c>
-      <c r="D59" t="s">
-        <v>110</v>
-      </c>
-      <c r="F59" t="s">
-        <v>87</v>
-      </c>
-      <c r="G59" t="s">
-        <v>89</v>
-      </c>
-      <c r="I59" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>70</v>
-      </c>
-      <c r="B60" t="s">
-        <v>111</v>
-      </c>
-      <c r="C60" t="s">
-        <v>98</v>
-      </c>
-      <c r="D60" t="s">
-        <v>132</v>
-      </c>
-      <c r="F60" t="s">
-        <v>87</v>
-      </c>
-      <c r="G60" t="s">
-        <v>89</v>
-      </c>
-      <c r="I60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>72</v>
-      </c>
-      <c r="B61" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" t="s">
-        <v>98</v>
-      </c>
-      <c r="D61" t="s">
-        <v>113</v>
-      </c>
-      <c r="F61" t="s">
-        <v>87</v>
-      </c>
-      <c r="G61" t="s">
-        <v>89</v>
-      </c>
-      <c r="I61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>73</v>
-      </c>
-      <c r="B62" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" t="s">
-        <v>98</v>
-      </c>
-      <c r="D62" t="s">
-        <v>110</v>
-      </c>
-      <c r="F62" t="s">
-        <v>87</v>
-      </c>
-      <c r="G62" t="s">
-        <v>89</v>
-      </c>
-      <c r="I62" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>71</v>
-      </c>
-      <c r="B63" t="s">
-        <v>116</v>
-      </c>
-      <c r="C63" t="s">
-        <v>113</v>
-      </c>
-      <c r="D63" t="s">
-        <v>88</v>
-      </c>
-      <c r="F63" t="s">
-        <v>87</v>
-      </c>
-      <c r="G63" t="s">
-        <v>89</v>
-      </c>
-      <c r="I63" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C65" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65" s="57" t="s">
+        <v>134</v>
+      </c>
       <c r="I65" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
+        <v>102</v>
+      </c>
+      <c r="C66" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" t="s">
+        <v>105</v>
+      </c>
+      <c r="F66" t="s">
+        <v>121</v>
+      </c>
+      <c r="G66" t="s">
+        <v>107</v>
+      </c>
+      <c r="I66" t="s">
         <v>110</v>
-      </c>
-      <c r="C66" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" t="s">
-        <v>113</v>
-      </c>
-      <c r="F66" t="s">
-        <v>129</v>
-      </c>
-      <c r="G66" t="s">
-        <v>115</v>
-      </c>
-      <c r="I66" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B67" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C67" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D67" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F67" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G67" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I67" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D68" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F68" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G68" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I68" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C69" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D69" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F69" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G69" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I69" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C70" t="s">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D70" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="F70" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G70" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I70" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C71" t="s">
+        <v>84</v>
+      </c>
+      <c r="D71" t="s">
+        <v>105</v>
+      </c>
+      <c r="F71" t="s">
+        <v>121</v>
+      </c>
+      <c r="G71" t="s">
+        <v>107</v>
+      </c>
+      <c r="I71" t="s">
         <v>113</v>
-      </c>
-      <c r="D71" t="s">
-        <v>92</v>
-      </c>
-      <c r="F71" t="s">
-        <v>129</v>
-      </c>
-      <c r="G71" t="s">
-        <v>115</v>
-      </c>
-      <c r="I71" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C75" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D75" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I75" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D76" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E76" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I76" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C77" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D77" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F77" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="G77" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I77" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made jade wine more interesting
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0459D5-76B9-4BF6-87AD-C93BC3E8E319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DD15AE-2389-4AE5-815E-EAC746E5D11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34395" yWindow="0" windowWidth="17205" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
+    <workbookView xWindow="25110" yWindow="0" windowWidth="26490" windowHeight="21000" activeTab="1" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Infused Beverages" sheetId="1" r:id="rId1"/>
+    <sheet name="Suspicious Brew" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="152">
   <si>
     <t>thickness</t>
   </si>
@@ -471,6 +472,24 @@
   </si>
   <si>
     <t>30 days</t>
+  </si>
+  <si>
+    <t>8x rice</t>
+  </si>
+  <si>
+    <t>sake</t>
+  </si>
+  <si>
+    <t>Alc %</t>
+  </si>
+  <si>
+    <t>Duration (ticks)</t>
+  </si>
+  <si>
+    <t>Duration (min)</t>
+  </si>
+  <si>
+    <t>Flower Effect Duration (ticks):</t>
   </si>
 </sst>
 </file>
@@ -519,7 +538,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -579,6 +598,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -851,7 +882,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -911,13 +942,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -976,11 +1058,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}" name="Tabelle1" displayName="Tabelle1" ref="A20:I39" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}" name="Tabelle1" displayName="Tabelle1" ref="A20:I39" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A20:I39" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{01EC8C57-83BE-4610-A43F-E9C497C3103A}" name="Beverage Type" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{3AFBF746-223D-4849-8D15-6B5EBC41CD07}" name="Ferm.Mod" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{01EC8C57-83BE-4610-A43F-E9C497C3103A}" name="Beverage Type" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{3AFBF746-223D-4849-8D15-6B5EBC41CD07}" name="Ferm.Mod" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{1E074399-223F-4717-8110-138418658072}" name="32">
       <calculatedColumnFormula>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
@@ -999,11 +1081,27 @@
     <tableColumn id="8" xr3:uid="{253E0318-1896-406A-A446-939D5EA3C3B1}" name="1008">
       <calculatedColumnFormula>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{1D17B4C3-392F-435C-82A2-4BFC2C15EC49}" name="2160" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{1D17B4C3-392F-435C-82A2-4BFC2C15EC49}" name="2160" dataDxfId="3">
       <calculatedColumnFormula>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0BF37B44-A763-428F-8551-939499375526}" name="Tabelle2" displayName="Tabelle2" ref="B4:D14" totalsRowShown="0" tableBorderDxfId="2">
+  <autoFilter ref="B4:D14" xr:uid="{0BF37B44-A763-428F-8551-939499375526}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{08376E7B-C222-4FBA-8483-E526978CB6C8}" name="Alc %"/>
+    <tableColumn id="2" xr3:uid="{6E624D1C-0B3E-46C4-A19C-0FD76E060EE6}" name="Duration (ticks)" dataDxfId="0">
+      <calculatedColumnFormula>POWER($D$3,1 + B5 *0.15)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{39FAC904-00AF-45C1-8287-CA356DB8CAFA}" name="Duration (min)" dataDxfId="1">
+      <calculatedColumnFormula>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1304,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B33BBD-CB27-4534-9864-9F1639537D70}">
-  <dimension ref="A1:Y77"/>
+  <dimension ref="A1:Y78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3041,16 +3139,16 @@
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>147</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C62" t="s">
         <v>90</v>
       </c>
       <c r="D62" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="F62" t="s">
         <v>79</v>
@@ -3059,21 +3157,21 @@
         <v>81</v>
       </c>
       <c r="I62" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
       <c r="C63" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D63" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="F63" t="s">
         <v>79</v>
@@ -3082,52 +3180,52 @@
         <v>81</v>
       </c>
       <c r="I63" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" t="s">
+        <v>105</v>
+      </c>
+      <c r="D64" t="s">
+        <v>80</v>
+      </c>
+      <c r="F64" t="s">
+        <v>79</v>
+      </c>
+      <c r="G64" t="s">
+        <v>81</v>
+      </c>
+      <c r="I64" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B65" s="57" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B66" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="C65" s="57" t="s">
+      <c r="C66" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="D65" s="57" t="s">
+      <c r="D66" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="I65" t="s">
+      <c r="I66" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66" t="s">
-        <v>102</v>
-      </c>
-      <c r="C66" t="s">
-        <v>92</v>
-      </c>
-      <c r="D66" t="s">
-        <v>105</v>
-      </c>
-      <c r="F66" t="s">
-        <v>121</v>
-      </c>
-      <c r="G66" t="s">
-        <v>107</v>
-      </c>
-      <c r="I66" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="C67" t="s">
         <v>92</v>
@@ -3142,15 +3240,15 @@
         <v>107</v>
       </c>
       <c r="I67" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C68" t="s">
         <v>92</v>
@@ -3165,15 +3263,15 @@
         <v>107</v>
       </c>
       <c r="I68" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C69" t="s">
         <v>92</v>
@@ -3188,18 +3286,18 @@
         <v>107</v>
       </c>
       <c r="I69" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="D70" t="s">
         <v>105</v>
@@ -3211,15 +3309,15 @@
         <v>107</v>
       </c>
       <c r="I70" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="C71" t="s">
         <v>84</v>
@@ -3234,37 +3332,43 @@
         <v>107</v>
       </c>
       <c r="I71" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>68</v>
+      </c>
+      <c r="B72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72" t="s">
+        <v>105</v>
+      </c>
+      <c r="F72" t="s">
+        <v>121</v>
+      </c>
+      <c r="G72" t="s">
+        <v>107</v>
+      </c>
+      <c r="I72" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>71</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>112</v>
-      </c>
-      <c r="C75" t="s">
-        <v>83</v>
-      </c>
-      <c r="D75" t="s">
-        <v>84</v>
-      </c>
-      <c r="I75" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
         <v>112</v>
@@ -3273,35 +3377,52 @@
         <v>83</v>
       </c>
       <c r="D76" t="s">
-        <v>105</v>
-      </c>
-      <c r="E76" t="s">
         <v>84</v>
       </c>
       <c r="I76" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D77" t="s">
+        <v>105</v>
+      </c>
+      <c r="E77" t="s">
+        <v>84</v>
+      </c>
+      <c r="I77" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>123</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>124</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>103</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F78" t="s">
         <v>130</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G78" t="s">
         <v>129</v>
       </c>
-      <c r="I77" t="s">
+      <c r="I78" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3348,4 +3469,191 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5590FB0-7861-4C68-9F7C-2BB835CA7538}">
+  <dimension ref="B1:D14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="61"/>
+      <c r="D2" s="62"/>
+    </row>
+    <row r="3" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="66"/>
+      <c r="D3" s="59">
+        <f>20*12*4</f>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="64">
+        <f>POWER($D$3,1 + B5 *0.1)</f>
+        <v>960</v>
+      </c>
+      <c r="D5" s="63">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="65">
+        <f t="shared" ref="C6:C14" si="0">POWER($D$3,1 + B6 *0.15)</f>
+        <v>7532.7335020499258</v>
+      </c>
+      <c r="D6" s="63">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>6.2772779183749376</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="65">
+        <f t="shared" si="0"/>
+        <v>59106.327096776331</v>
+      </c>
+      <c r="D7" s="63">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>49.255272580646945</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="65">
+        <f t="shared" si="0"/>
+        <v>463783.55240104912</v>
+      </c>
+      <c r="D8" s="63">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>386.48629366754091</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="65">
+        <f t="shared" si="0"/>
+        <v>3639122.8154907427</v>
+      </c>
+      <c r="D9" s="63">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>3032.6023462422859</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="3">
+        <v>9</v>
+      </c>
+      <c r="C10" s="65">
+        <f t="shared" si="0"/>
+        <v>10193830.257075245</v>
+      </c>
+      <c r="D10" s="63">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>8494.8585475627042</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="3">
+        <v>19</v>
+      </c>
+      <c r="C11" s="65">
+        <f t="shared" si="0"/>
+        <v>303210507415.43286</v>
+      </c>
+      <c r="D11" s="63">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>252675422.84619406</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>11</v>
+      </c>
+      <c r="C12" s="64">
+        <f t="shared" si="0"/>
+        <v>79986881.970500872</v>
+      </c>
+      <c r="D12" s="63">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>66655.734975417392</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="67">
+        <v>12</v>
+      </c>
+      <c r="C13" s="68">
+        <f t="shared" si="0"/>
+        <v>224057482.78930962</v>
+      </c>
+      <c r="D13" s="69">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>186714.56899109136</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="67">
+        <v>15</v>
+      </c>
+      <c r="C14" s="68">
+        <f t="shared" si="0"/>
+        <v>4924719592.9163141</v>
+      </c>
+      <c r="D14" s="69">
+        <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
+        <v>4103932.9940969283</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
lots of new foods + drinks
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DD15AE-2389-4AE5-815E-EAC746E5D11D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B6F312-6BA3-4BD2-89D5-D7F3851F02F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25110" yWindow="0" windowWidth="26490" windowHeight="21000" activeTab="1" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
+    <workbookView xWindow="15285" yWindow="0" windowWidth="36315" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Infused Beverages" sheetId="1" r:id="rId1"/>
@@ -21,20 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="157">
   <si>
     <t>thickness</t>
   </si>
@@ -186,9 +178,6 @@
     <t>(nectar multiplies days by 1.5 and dampens negative effects)</t>
   </si>
   <si>
-    <t>berry_liquor, glow_berry_liquor, advocaat, mint_cream, hare_bane_creme, incubus_cream, mead, artemisa</t>
-  </si>
-  <si>
     <t>Non Alcoholic</t>
   </si>
   <si>
@@ -490,6 +479,24 @@
   </si>
   <si>
     <t>Flower Effect Duration (ticks):</t>
+  </si>
+  <si>
+    <t>myceylon_liquor</t>
+  </si>
+  <si>
+    <t>myceylon, sugar</t>
+  </si>
+  <si>
+    <t>mullet_wine</t>
+  </si>
+  <si>
+    <t>immunity</t>
+  </si>
+  <si>
+    <t>berry_liquor, glow_berry_liquor, myceylon_liquor, advocaat, mint_cream, hare_bane_creme, incubus_cream, mead, artemisa, mullet_wine</t>
+  </si>
+  <si>
+    <t>sweet_berries, myceylon, prickly_bayleaf, moonstruck_nectar</t>
   </si>
 </sst>
 </file>
@@ -882,15 +889,12 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -922,16 +926,15 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
@@ -943,6 +946,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -950,23 +967,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -977,11 +977,11 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1094,10 +1094,10 @@
   <autoFilter ref="B4:D14" xr:uid="{0BF37B44-A763-428F-8551-939499375526}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{08376E7B-C222-4FBA-8483-E526978CB6C8}" name="Alc %"/>
-    <tableColumn id="2" xr3:uid="{6E624D1C-0B3E-46C4-A19C-0FD76E060EE6}" name="Duration (ticks)" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{6E624D1C-0B3E-46C4-A19C-0FD76E060EE6}" name="Duration (ticks)" dataDxfId="1">
       <calculatedColumnFormula>POWER($D$3,1 + B5 *0.15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{39FAC904-00AF-45C1-8287-CA356DB8CAFA}" name="Duration (min)" dataDxfId="1">
+    <tableColumn id="3" xr3:uid="{39FAC904-00AF-45C1-8287-CA356DB8CAFA}" name="Duration (min)" dataDxfId="0">
       <calculatedColumnFormula>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1402,10 +1402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B33BBD-CB27-4534-9864-9F1639537D70}">
-  <dimension ref="A1:Y78"/>
+  <dimension ref="A1:Y80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1419,15 +1419,15 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="26">
         <v>18</v>
       </c>
       <c r="D3" t="s">
@@ -1435,10 +1435,10 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="27">
         <v>2</v>
       </c>
       <c r="C4"/>
@@ -1456,75 +1456,74 @@
       <c r="M4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="28">
         <v>18</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="20">
         <v>18</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="20">
         <v>18</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="20">
         <v>18</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>18</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>18</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="20">
         <v>18</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="20">
         <v>18</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="20">
         <v>18</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="20">
         <v>18</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="20">
         <v>18</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="21">
         <v>18</v>
       </c>
       <c r="O7" t="s">
@@ -1532,43 +1531,43 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="29">
         <v>72</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="22">
         <v>144</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <v>196</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="22">
         <v>196</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>196</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="22">
         <v>72</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="22">
         <v>72</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="22">
         <v>72</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="22">
         <v>72</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K8" s="22">
         <v>72</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="22">
         <v>72</v>
       </c>
-      <c r="M8" s="26">
+      <c r="M8" s="23">
         <v>72</v>
       </c>
       <c r="O8" t="s">
@@ -1576,43 +1575,43 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="30">
         <v>0.4</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="24">
         <v>0.4</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="24">
         <v>0.4</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="24">
         <v>1</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="24">
         <v>0</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="24">
         <v>0.4</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="24">
         <v>0.4</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="24">
         <v>0.4</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="24">
         <v>0.4</v>
       </c>
-      <c r="K9" s="27">
+      <c r="K9" s="24">
         <v>0.4</v>
       </c>
-      <c r="L9" s="27">
+      <c r="L9" s="24">
         <v>0.4</v>
       </c>
-      <c r="M9" s="28">
+      <c r="M9" s="25">
         <v>0.4</v>
       </c>
       <c r="O9" t="s">
@@ -1620,86 +1619,85 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="31">
         <f>B8*3</f>
         <v>216</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="13">
         <f t="shared" ref="C12:M12" si="0">C8*3</f>
         <v>432</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="13">
         <f t="shared" si="0"/>
         <v>588</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="13">
         <f t="shared" si="0"/>
         <v>588</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="13">
         <f t="shared" si="0"/>
         <v>588</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="13">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="13">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="13">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="13">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="13">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="13">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="M12" s="17">
+      <c r="M12" s="14">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
@@ -1708,54 +1706,54 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="32">
         <f>B7/$B$3</f>
         <v>1</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="15">
         <f t="shared" ref="C13:M13" si="1">C7/$B$3</f>
         <v>1</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="16">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1764,54 +1762,54 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="33">
         <f>IF($B$4=0,0,LOG(B12*(0.5+B13/2)*(0.5+B9/2),1+$B$4)/100)</f>
         <v>4.5681297355864098E-2</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="17">
         <f t="shared" ref="C14:M14" si="2">IF($B$4=0,0,LOG(C12*(0.5+C13/2)*(0.5+C9/2),1+$B$4)/100)</f>
         <v>5.1990594891578673E-2</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="17">
         <f t="shared" si="2"/>
         <v>5.4796874803377964E-2</v>
       </c>
-      <c r="E14" s="20">
+      <c r="E14" s="17">
         <f t="shared" si="2"/>
         <v>5.8043470054657584E-2</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="17">
         <f t="shared" si="2"/>
         <v>5.1734172518943015E-2</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="17">
         <f t="shared" si="2"/>
         <v>4.5681297355864098E-2</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="17">
         <f t="shared" si="2"/>
         <v>4.5681297355864098E-2</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="17">
         <f t="shared" si="2"/>
         <v>4.5681297355864098E-2</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="17">
         <f t="shared" si="2"/>
         <v>4.5681297355864098E-2</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14" s="17">
         <f t="shared" si="2"/>
         <v>4.5681297355864098E-2</v>
       </c>
-      <c r="L14" s="20">
+      <c r="L14" s="17">
         <f t="shared" si="2"/>
         <v>4.5681297355864098E-2</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M14" s="18">
         <f t="shared" si="2"/>
         <v>4.5681297355864098E-2</v>
       </c>
@@ -1820,54 +1818,54 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="19">
         <f>ABS(1.5-B13/2)</f>
         <v>1</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="19">
         <f>ABS(1.5-C13/2)</f>
         <v>1</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="19">
         <f t="shared" ref="D15:M15" si="3">ABS(1.5-D13/2)</f>
         <v>1</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K15" s="22">
+      <c r="K15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L15" s="22">
+      <c r="L15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="19">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -1875,183 +1873,159 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49" t="s">
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43" t="s">
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="45">
+      <c r="F18" s="41">
         <v>1</v>
       </c>
-      <c r="G18" s="43" t="s">
+      <c r="G18" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="45">
+      <c r="H18" s="41">
         <v>0.4</v>
       </c>
-      <c r="I18" s="44"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47" t="s">
+      <c r="I18" s="40"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="42"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="47" t="s">
+      <c r="F19" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="47" t="s">
+      <c r="G19" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
+        <v>140</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>139</v>
+      </c>
+      <c r="F20" t="s">
+        <v>138</v>
+      </c>
+      <c r="G20" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="H20" t="s">
         <v>142</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="I20" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="I20" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="J20" s="3"/>
       <c r="K20" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" t="s">
         <v>43</v>
       </c>
-      <c r="M20" s="3"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="54">
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="50">
         <v>0</v>
       </c>
-      <c r="C21" s="52">
+      <c r="C21" s="48">
         <v>0</v>
       </c>
-      <c r="D21" s="52">
+      <c r="D21" s="48">
         <v>0</v>
       </c>
-      <c r="E21" s="52">
+      <c r="E21" s="48">
         <v>0</v>
       </c>
-      <c r="F21" s="52">
+      <c r="F21" s="48">
         <v>0</v>
       </c>
-      <c r="G21" s="52">
+      <c r="G21" s="48">
         <v>0</v>
       </c>
-      <c r="H21" s="52">
+      <c r="H21" s="48">
         <v>0</v>
       </c>
-      <c r="I21" s="53">
+      <c r="I21" s="49">
         <v>0</v>
       </c>
-      <c r="J21" s="3"/>
       <c r="K21">
         <v>4</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L21" t="s">
         <v>34</v>
       </c>
-      <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="39" t="s">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="55">
+      <c r="B22" s="51">
         <v>1.25</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
         <v>3.833943903789129E-2</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
         <v>4.8339439037891292E-2</v>
       </c>
-      <c r="E22" s="40">
+      <c r="E22" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
         <v>5.6886995494648568E-2</v>
       </c>
-      <c r="F22" s="40">
+      <c r="F22" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
         <v>6.1886995494648572E-2</v>
       </c>
-      <c r="G22" s="40">
+      <c r="G22" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
         <v>6.543455195140585E-2</v>
       </c>
-      <c r="H22" s="40">
+      <c r="H22" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
         <v>8.0883020185091359E-2</v>
       </c>
-      <c r="I22" s="41">
+      <c r="I22" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
         <v>9.028136343098643E-2</v>
       </c>
@@ -2062,38 +2036,38 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="39" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="55">
+      <c r="B23" s="51">
         <v>1.25</v>
       </c>
-      <c r="C23" s="40">
+      <c r="C23" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
         <v>3.833943903789129E-2</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
         <v>4.8339439037891292E-2</v>
       </c>
-      <c r="E23" s="40">
+      <c r="E23" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
         <v>5.6886995494648568E-2</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
         <v>6.1886995494648572E-2</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
         <v>6.543455195140585E-2</v>
       </c>
-      <c r="H23" s="40">
+      <c r="H23" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
         <v>8.0883020185091359E-2</v>
       </c>
-      <c r="I23" s="41">
+      <c r="I23" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
         <v>9.028136343098643E-2</v>
       </c>
@@ -2104,38 +2078,38 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="55">
+      <c r="B24" s="51">
         <v>0.25</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
         <v>0.13933008328271637</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
         <v>0.17567127313294212</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
         <v>0.20673411032799602</v>
       </c>
-      <c r="F24" s="40">
+      <c r="F24" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
         <v>0.22490470525310891</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
         <v>0.23779694752304992</v>
       </c>
-      <c r="H24" s="40">
+      <c r="H24" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
         <v>0.2939385192206046</v>
       </c>
-      <c r="I24" s="41">
+      <c r="I24" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
         <v>0.32809321683827058</v>
       </c>
@@ -2143,41 +2117,41 @@
         <v>24</v>
       </c>
       <c r="L24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="55">
+      <c r="B25" s="51">
         <v>0.125</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
         <v>0.26396508983953099</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
         <v>0.33281458176314815</v>
       </c>
-      <c r="E25" s="40">
+      <c r="E25" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
         <v>0.39166407368676537</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
         <v>0.42608881964857398</v>
       </c>
-      <c r="G25" s="40">
+      <c r="G25" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
         <v>0.45051356561038253</v>
       </c>
-      <c r="H25" s="40">
+      <c r="H25" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
         <v>0.55687548449912128</v>
       </c>
-      <c r="I25" s="41">
+      <c r="I25" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
         <v>0.62158260023948475</v>
       </c>
@@ -2185,201 +2159,201 @@
         <v>24</v>
       </c>
       <c r="L25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="40" t="str">
+      <c r="B26" s="51"/>
+      <c r="C26" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
-      <c r="D26" s="40" t="str">
+      <c r="D26" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
-      <c r="E26" s="40" t="str">
+      <c r="E26" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
-      <c r="F26" s="40" t="str">
+      <c r="F26" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
-      <c r="G26" s="40" t="str">
+      <c r="G26" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
-      <c r="H26" s="40" t="str">
+      <c r="H26" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
-      <c r="I26" s="41" t="str">
+      <c r="I26" s="37" t="str">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="40" t="str">
+      <c r="B27" s="51"/>
+      <c r="C27" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
-      <c r="D27" s="40" t="str">
+      <c r="D27" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
-      <c r="E27" s="40" t="str">
+      <c r="E27" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
-      <c r="F27" s="40" t="str">
+      <c r="F27" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
-      <c r="G27" s="40" t="str">
+      <c r="G27" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
-      <c r="H27" s="40" t="str">
+      <c r="H27" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
-      <c r="I27" s="41" t="str">
+      <c r="I27" s="37" t="str">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="40" t="str">
+      <c r="B28" s="51"/>
+      <c r="C28" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
-      <c r="D28" s="40" t="str">
+      <c r="D28" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
-      <c r="E28" s="40" t="str">
+      <c r="E28" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
-      <c r="F28" s="40" t="str">
+      <c r="F28" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
-      <c r="G28" s="40" t="str">
+      <c r="G28" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
-      <c r="H28" s="40" t="str">
+      <c r="H28" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
-      <c r="I28" s="41" t="str">
+      <c r="I28" s="37" t="str">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="40" t="str">
+      <c r="B29" s="51"/>
+      <c r="C29" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
-      <c r="D29" s="40" t="str">
+      <c r="D29" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
-      <c r="E29" s="40" t="str">
+      <c r="E29" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
-      <c r="F29" s="40" t="str">
+      <c r="F29" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
-      <c r="G29" s="40" t="str">
+      <c r="G29" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
-      <c r="H29" s="40" t="str">
+      <c r="H29" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
-      <c r="I29" s="41" t="str">
+      <c r="I29" s="37" t="str">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="40" t="str">
+      <c r="B30" s="51"/>
+      <c r="C30" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
-      <c r="D30" s="40" t="str">
+      <c r="D30" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
-      <c r="E30" s="40" t="str">
+      <c r="E30" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
-      <c r="F30" s="40" t="str">
+      <c r="F30" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
-      <c r="G30" s="40" t="str">
+      <c r="G30" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
-      <c r="H30" s="40" t="str">
+      <c r="H30" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
-      <c r="I30" s="41" t="str">
+      <c r="I30" s="37" t="str">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="55">
+      <c r="B31" s="51">
         <v>0.1</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C31" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
         <v>0.32620450042629268</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
         <v>0.41128777462441041</v>
       </c>
-      <c r="E31" s="40">
+      <c r="E31" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
         <v>0.48401318359782758</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
         <v>0.52655482069688653</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
         <v>0.55673859257124469</v>
       </c>
-      <c r="H31" s="40">
+      <c r="H31" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
         <v>0.68817921843800245</v>
       </c>
-      <c r="I31" s="41">
+      <c r="I31" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
         <v>0.76814339997785419</v>
       </c>
@@ -2387,38 +2361,38 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="55">
+      <c r="B32" s="51">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C32" s="40">
+      <c r="C32" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
         <v>0.42989940785288216</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
         <v>0.54202921951444771</v>
       </c>
-      <c r="E32" s="40">
+      <c r="E32" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
         <v>0.63787280908072685</v>
       </c>
-      <c r="F32" s="40">
+      <c r="F32" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
         <v>0.69393771491150957</v>
       </c>
-      <c r="G32" s="40">
+      <c r="G32" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
         <v>0.733716398647006</v>
       </c>
-      <c r="H32" s="40">
+      <c r="H32" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
         <v>0.90693978199728931</v>
       </c>
-      <c r="I32" s="41">
+      <c r="I32" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
         <v>1.0123232278065855</v>
       </c>
@@ -2430,34 +2404,34 @@
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="55">
+      <c r="B33" s="51">
         <v>0.25</v>
       </c>
-      <c r="C33" s="40">
+      <c r="C33" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
         <v>0.13933008328271637</v>
       </c>
-      <c r="D33" s="40">
+      <c r="D33" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
         <v>0.17567127313294212</v>
       </c>
-      <c r="E33" s="40">
+      <c r="E33" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
         <v>0.20673411032799602</v>
       </c>
-      <c r="F33" s="40">
+      <c r="F33" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
         <v>0.22490470525310891</v>
       </c>
-      <c r="G33" s="40">
+      <c r="G33" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
         <v>0.23779694752304992</v>
       </c>
-      <c r="H33" s="40">
+      <c r="H33" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
         <v>0.2939385192206046</v>
       </c>
-      <c r="I33" s="41">
+      <c r="I33" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
         <v>0.32809321683827058</v>
       </c>
@@ -2469,34 +2443,34 @@
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="55">
+      <c r="B34" s="51">
         <v>0.5</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
         <v>7.6678878075782581E-2</v>
       </c>
-      <c r="D34" s="40">
+      <c r="D34" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
         <v>9.6678878075782584E-2</v>
       </c>
-      <c r="E34" s="40">
+      <c r="E34" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
         <v>0.11377399098929714</v>
       </c>
-      <c r="F34" s="40">
+      <c r="F34" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
         <v>0.12377399098929714</v>
       </c>
-      <c r="G34" s="40">
+      <c r="G34" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
         <v>0.1308691039028117</v>
       </c>
-      <c r="H34" s="40">
+      <c r="H34" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
         <v>0.16176604037018272</v>
       </c>
-      <c r="I34" s="41">
+      <c r="I34" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
         <v>0.18056272686197286</v>
       </c>
@@ -2508,34 +2482,34 @@
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="55">
+      <c r="B35" s="51">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
         <v>0.42989940785288216</v>
       </c>
-      <c r="D35" s="40">
+      <c r="D35" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
         <v>0.54202921951444771</v>
       </c>
-      <c r="E35" s="40">
+      <c r="E35" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
         <v>0.63787280908072685</v>
       </c>
-      <c r="F35" s="40">
+      <c r="F35" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
         <v>0.69393771491150957</v>
       </c>
-      <c r="G35" s="40">
+      <c r="G35" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
         <v>0.733716398647006</v>
       </c>
-      <c r="H35" s="40">
+      <c r="H35" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
         <v>0.90693978199728931</v>
       </c>
-      <c r="I35" s="41">
+      <c r="I35" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
         <v>1.0123232278065855</v>
       </c>
@@ -2550,34 +2524,34 @@
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="55">
+      <c r="B36" s="51">
         <v>1</v>
       </c>
-      <c r="C36" s="40">
+      <c r="C36" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
         <v>4.485426827170242E-2</v>
       </c>
-      <c r="D36" s="40">
+      <c r="D36" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
         <v>5.6553518286125544E-2</v>
       </c>
-      <c r="E36" s="40">
+      <c r="E36" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
         <v>6.6553518286125546E-2</v>
       </c>
-      <c r="F36" s="40">
+      <c r="F36" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
         <v>7.2403143293337108E-2</v>
       </c>
-      <c r="G36" s="40">
+      <c r="G36" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
         <v>7.6553518286125541E-2</v>
       </c>
-      <c r="H36" s="40">
+      <c r="H36" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
         <v>9.4627067506701593E-2</v>
       </c>
-      <c r="I36" s="41">
+      <c r="I36" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
         <v>0.10562242424221072</v>
       </c>
@@ -2587,100 +2561,100 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B37" s="55">
+        <v>136</v>
+      </c>
+      <c r="B37" s="51">
         <v>1</v>
       </c>
-      <c r="C37" s="40">
+      <c r="C37" s="36">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
         <v>4.485426827170242E-2</v>
       </c>
-      <c r="D37" s="40">
+      <c r="D37" s="36">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
         <v>5.6553518286125544E-2</v>
       </c>
-      <c r="E37" s="40">
+      <c r="E37" s="36">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
         <v>6.6553518286125546E-2</v>
       </c>
-      <c r="F37" s="40">
+      <c r="F37" s="36">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
         <v>7.2403143293337108E-2</v>
       </c>
-      <c r="G37" s="40">
+      <c r="G37" s="36">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
         <v>7.6553518286125541E-2</v>
       </c>
-      <c r="H37" s="40">
+      <c r="H37" s="36">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
         <v>9.4627067506701593E-2</v>
       </c>
-      <c r="I37" s="41">
+      <c r="I37" s="37">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
         <v>0.10562242424221072</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="40" t="str">
+      <c r="B38" s="51"/>
+      <c r="C38" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
-      <c r="D38" s="40" t="str">
+      <c r="D38" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
-      <c r="E38" s="40" t="str">
+      <c r="E38" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
-      <c r="F38" s="40" t="str">
+      <c r="F38" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
-      <c r="G38" s="40" t="str">
+      <c r="G38" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
-      <c r="H38" s="40" t="str">
+      <c r="H38" s="36" t="str">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
-      <c r="I38" s="41" t="str">
+      <c r="I38" s="37" t="str">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
-      <c r="B39" s="56"/>
-      <c r="C39" s="50" t="str">
+      <c r="A39" s="38"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="46" t="str">
         <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
-      <c r="D39" s="50" t="str">
+      <c r="D39" s="46" t="str">
         <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
-      <c r="E39" s="50" t="str">
+      <c r="E39" s="46" t="str">
         <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
-      <c r="F39" s="50" t="str">
+      <c r="F39" s="46" t="str">
         <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
-      <c r="G39" s="50" t="str">
+      <c r="G39" s="46" t="str">
         <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
-      <c r="H39" s="50" t="str">
+      <c r="H39" s="46" t="str">
         <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
-      <c r="I39" s="51" t="str">
+      <c r="I39" s="47" t="str">
         <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
         <v/>
       </c>
@@ -2690,577 +2664,588 @@
         <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I42" t="s">
-        <v>89</v>
-      </c>
-      <c r="S42" s="58"/>
-      <c r="T42" s="58"/>
-      <c r="U42" s="58"/>
-      <c r="V42" s="58"/>
-      <c r="W42" s="58"/>
-      <c r="X42" s="58"/>
-      <c r="Y42" s="58"/>
+        <v>88</v>
+      </c>
+      <c r="S42" s="54"/>
+      <c r="T42" s="54"/>
+      <c r="U42" s="54"/>
+      <c r="V42" s="54"/>
+      <c r="W42" s="54"/>
+      <c r="X42" s="54"/>
+      <c r="Y42" s="54"/>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" t="s">
         <v>76</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F43" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" t="s">
         <v>77</v>
       </c>
-      <c r="F43" t="s">
-        <v>131</v>
-      </c>
-      <c r="G43" t="s">
-        <v>78</v>
-      </c>
       <c r="I43" t="s">
-        <v>86</v>
-      </c>
-      <c r="S43" s="58"/>
-      <c r="T43" s="58"/>
-      <c r="U43" s="58"/>
-      <c r="V43" s="58"/>
-      <c r="W43" s="58"/>
-      <c r="X43" s="58"/>
-      <c r="Y43" s="58"/>
+        <v>85</v>
+      </c>
+      <c r="S43" s="54"/>
+      <c r="T43" s="54"/>
+      <c r="U43" s="54"/>
+      <c r="V43" s="54"/>
+      <c r="W43" s="54"/>
+      <c r="X43" s="54"/>
+      <c r="Y43" s="54"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" t="s">
         <v>76</v>
       </c>
-      <c r="D44" t="s">
+      <c r="F44" t="s">
+        <v>130</v>
+      </c>
+      <c r="G44" t="s">
         <v>77</v>
       </c>
-      <c r="F44" t="s">
-        <v>131</v>
-      </c>
-      <c r="G44" t="s">
-        <v>78</v>
-      </c>
       <c r="I44" t="s">
-        <v>85</v>
-      </c>
-      <c r="S44" s="58"/>
-      <c r="T44" s="58"/>
-      <c r="U44" s="58"/>
-      <c r="V44" s="58"/>
-      <c r="W44" s="58"/>
-      <c r="X44" s="58"/>
-      <c r="Y44" s="58"/>
+        <v>84</v>
+      </c>
+      <c r="S44" s="54"/>
+      <c r="T44" s="54"/>
+      <c r="U44" s="54"/>
+      <c r="V44" s="54"/>
+      <c r="W44" s="54"/>
+      <c r="X44" s="54"/>
+      <c r="Y44" s="54"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" t="s">
         <v>76</v>
       </c>
-      <c r="D45" t="s">
+      <c r="F45" t="s">
+        <v>130</v>
+      </c>
+      <c r="G45" t="s">
         <v>77</v>
       </c>
-      <c r="F45" t="s">
-        <v>131</v>
-      </c>
-      <c r="G45" t="s">
-        <v>78</v>
-      </c>
       <c r="I45" t="s">
-        <v>87</v>
-      </c>
-      <c r="S45" s="58"/>
-      <c r="T45" s="58"/>
-      <c r="U45" s="58"/>
-      <c r="V45" s="58"/>
-      <c r="W45" s="58"/>
-      <c r="X45" s="58"/>
-      <c r="Y45" s="58"/>
+        <v>86</v>
+      </c>
+      <c r="S45" s="54"/>
+      <c r="T45" s="54"/>
+      <c r="U45" s="54"/>
+      <c r="V45" s="54"/>
+      <c r="W45" s="54"/>
+      <c r="X45" s="54"/>
+      <c r="Y45" s="54"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" t="s">
         <v>76</v>
       </c>
-      <c r="D46" t="s">
+      <c r="F46" t="s">
+        <v>130</v>
+      </c>
+      <c r="G46" t="s">
         <v>77</v>
       </c>
-      <c r="F46" t="s">
-        <v>131</v>
-      </c>
-      <c r="G46" t="s">
-        <v>78</v>
-      </c>
       <c r="I46" t="s">
-        <v>88</v>
-      </c>
-      <c r="S46" s="58"/>
-      <c r="T46" s="58"/>
-      <c r="U46" s="58"/>
-      <c r="V46" s="58"/>
-      <c r="W46" s="58"/>
-      <c r="X46" s="58"/>
-      <c r="Y46" s="58"/>
+        <v>87</v>
+      </c>
+      <c r="S46" s="54"/>
+      <c r="T46" s="54"/>
+      <c r="U46" s="54"/>
+      <c r="V46" s="54"/>
+      <c r="W46" s="54"/>
+      <c r="X46" s="54"/>
+      <c r="Y46" s="54"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S47" s="58"/>
-      <c r="T47" s="58"/>
-      <c r="U47" s="58"/>
-      <c r="V47" s="58"/>
-      <c r="W47" s="58"/>
-      <c r="X47" s="58"/>
-      <c r="Y47" s="58"/>
+      <c r="S47" s="54"/>
+      <c r="T47" s="54"/>
+      <c r="U47" s="54"/>
+      <c r="V47" s="54"/>
+      <c r="W47" s="54"/>
+      <c r="X47" s="54"/>
+      <c r="Y47" s="54"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I48" t="s">
-        <v>116</v>
-      </c>
-      <c r="S48" s="58"/>
-      <c r="T48" s="58"/>
-      <c r="U48" s="58"/>
-      <c r="V48" s="58"/>
-      <c r="W48" s="58"/>
-      <c r="X48" s="58"/>
-      <c r="Y48" s="58"/>
+        <v>115</v>
+      </c>
+      <c r="S48" s="54"/>
+      <c r="T48" s="54"/>
+      <c r="U48" s="54"/>
+      <c r="V48" s="54"/>
+      <c r="W48" s="54"/>
+      <c r="X48" s="54"/>
+      <c r="Y48" s="54"/>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>36</v>
       </c>
       <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
         <v>90</v>
       </c>
-      <c r="C49" t="s">
-        <v>91</v>
-      </c>
       <c r="F49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I49" t="s">
-        <v>94</v>
-      </c>
-      <c r="S49" s="58"/>
-      <c r="T49" s="58"/>
-      <c r="U49" s="58"/>
-      <c r="V49" s="58"/>
-      <c r="W49" s="58"/>
-      <c r="X49" s="58"/>
-      <c r="Y49" s="58"/>
+        <v>93</v>
+      </c>
+      <c r="S49" s="54"/>
+      <c r="T49" s="54"/>
+      <c r="U49" s="54"/>
+      <c r="V49" s="54"/>
+      <c r="W49" s="54"/>
+      <c r="X49" s="54"/>
+      <c r="Y49" s="54"/>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I50" t="s">
-        <v>95</v>
-      </c>
-      <c r="S50" s="58"/>
-      <c r="T50" s="58"/>
-      <c r="U50" s="58"/>
-      <c r="V50" s="58"/>
-      <c r="W50" s="58"/>
-      <c r="X50" s="58"/>
-      <c r="Y50" s="58"/>
+        <v>94</v>
+      </c>
+      <c r="S50" s="54"/>
+      <c r="T50" s="54"/>
+      <c r="U50" s="54"/>
+      <c r="V50" s="54"/>
+      <c r="W50" s="54"/>
+      <c r="X50" s="54"/>
+      <c r="Y50" s="54"/>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" t="s">
         <v>92</v>
       </c>
-      <c r="C51" t="s">
-        <v>91</v>
-      </c>
-      <c r="D51" t="s">
-        <v>93</v>
-      </c>
       <c r="F51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I51" t="s">
-        <v>96</v>
-      </c>
-      <c r="S51" s="58"/>
-      <c r="T51" s="58"/>
-      <c r="U51" s="58"/>
-      <c r="V51" s="58"/>
-      <c r="W51" s="58"/>
-      <c r="X51" s="58"/>
-      <c r="Y51" s="58"/>
+        <v>95</v>
+      </c>
+      <c r="S51" s="54"/>
+      <c r="T51" s="54"/>
+      <c r="U51" s="54"/>
+      <c r="V51" s="54"/>
+      <c r="W51" s="54"/>
+      <c r="X51" s="54"/>
+      <c r="Y51" s="54"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S52" s="58"/>
-      <c r="T52" s="58"/>
-      <c r="U52" s="58"/>
-      <c r="V52" s="58"/>
-      <c r="W52" s="58"/>
-      <c r="X52" s="58"/>
-      <c r="Y52" s="58"/>
+      <c r="S52" s="54"/>
+      <c r="T52" s="54"/>
+      <c r="U52" s="54"/>
+      <c r="V52" s="54"/>
+      <c r="W52" s="54"/>
+      <c r="X52" s="54"/>
+      <c r="Y52" s="54"/>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I53" t="s">
-        <v>117</v>
-      </c>
-      <c r="S53" s="58"/>
-      <c r="T53" s="58"/>
-      <c r="U53" s="58"/>
-      <c r="V53" s="58"/>
-      <c r="W53" s="58"/>
-      <c r="X53" s="58"/>
-      <c r="Y53" s="58"/>
+        <v>116</v>
+      </c>
+      <c r="S53" s="54"/>
+      <c r="T53" s="54"/>
+      <c r="U53" s="54"/>
+      <c r="V53" s="54"/>
+      <c r="W53" s="54"/>
+      <c r="X53" s="54"/>
+      <c r="Y53" s="54"/>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F54" t="s">
+        <v>78</v>
+      </c>
+      <c r="G54" t="s">
+        <v>77</v>
+      </c>
+      <c r="I54" t="s">
         <v>127</v>
       </c>
-      <c r="B54" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" t="s">
-        <v>90</v>
-      </c>
-      <c r="F54" t="s">
-        <v>79</v>
-      </c>
-      <c r="G54" t="s">
-        <v>78</v>
-      </c>
-      <c r="I54" t="s">
-        <v>128</v>
-      </c>
-      <c r="S54" s="58"/>
-      <c r="T54" s="58"/>
-      <c r="U54" s="58"/>
-      <c r="V54" s="58"/>
-      <c r="W54" s="58"/>
-      <c r="X54" s="58"/>
-      <c r="Y54" s="58"/>
+      <c r="S54" s="54"/>
+      <c r="T54" s="54"/>
+      <c r="U54" s="54"/>
+      <c r="V54" s="54"/>
+      <c r="W54" s="54"/>
+      <c r="X54" s="54"/>
+      <c r="Y54" s="54"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I55" t="s">
-        <v>97</v>
-      </c>
-      <c r="S55" s="58"/>
-      <c r="T55" s="58"/>
-      <c r="U55" s="58"/>
-      <c r="V55" s="58"/>
-      <c r="W55" s="58"/>
-      <c r="X55" s="58"/>
-      <c r="Y55" s="58"/>
+        <v>96</v>
+      </c>
+      <c r="S55" s="54"/>
+      <c r="T55" s="54"/>
+      <c r="U55" s="54"/>
+      <c r="V55" s="54"/>
+      <c r="W55" s="54"/>
+      <c r="X55" s="54"/>
+      <c r="Y55" s="54"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" t="s">
         <v>92</v>
       </c>
-      <c r="C56" t="s">
-        <v>90</v>
-      </c>
-      <c r="D56" t="s">
-        <v>93</v>
-      </c>
       <c r="F56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G56" t="s">
+        <v>77</v>
+      </c>
+      <c r="I56" t="s">
+        <v>97</v>
+      </c>
+      <c r="S56" s="54"/>
+      <c r="T56" s="54"/>
+      <c r="U56" s="54"/>
+      <c r="V56" s="54"/>
+      <c r="W56" s="54"/>
+      <c r="X56" s="54"/>
+      <c r="Y56" s="54"/>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" t="s">
         <v>78</v>
       </c>
-      <c r="I56" t="s">
-        <v>98</v>
-      </c>
-      <c r="S56" s="58"/>
-      <c r="T56" s="58"/>
-      <c r="U56" s="58"/>
-      <c r="V56" s="58"/>
-      <c r="W56" s="58"/>
-      <c r="X56" s="58"/>
-      <c r="Y56" s="58"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S57" s="58"/>
-      <c r="T57" s="58"/>
-      <c r="U57" s="58"/>
-      <c r="V57" s="58"/>
-      <c r="W57" s="58"/>
-      <c r="X57" s="58"/>
-      <c r="Y57" s="58"/>
+      <c r="G57" t="s">
+        <v>77</v>
+      </c>
+      <c r="I57" t="s">
+        <v>152</v>
+      </c>
+      <c r="S57" s="54"/>
+      <c r="T57" s="54"/>
+      <c r="U57" s="54"/>
+      <c r="V57" s="54"/>
+      <c r="W57" s="54"/>
+      <c r="X57" s="54"/>
+      <c r="Y57" s="54"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" t="s">
-        <v>105</v>
-      </c>
-      <c r="F58" t="s">
-        <v>79</v>
-      </c>
-      <c r="G58" t="s">
-        <v>81</v>
-      </c>
-      <c r="I58" t="s">
-        <v>132</v>
-      </c>
+      <c r="S58" s="54"/>
+      <c r="T58" s="54"/>
+      <c r="U58" s="54"/>
+      <c r="V58" s="54"/>
+      <c r="W58" s="54"/>
+      <c r="X58" s="54"/>
+      <c r="Y58" s="54"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>153</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C59" t="s">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="D59" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I59" t="s">
-        <v>99</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="S59" s="54"/>
+      <c r="T59" s="54"/>
+      <c r="U59" s="54"/>
+      <c r="V59" s="54"/>
+      <c r="W59" s="54"/>
+      <c r="X59" s="54"/>
+      <c r="Y59" s="54"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="D60" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="F60" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I60" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C61" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D61" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="F61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G61" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I61" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C62" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D62" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="F62" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G62" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I62" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="C63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" t="s">
         <v>90</v>
       </c>
-      <c r="D63" t="s">
-        <v>102</v>
-      </c>
       <c r="F63" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I63" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="B64" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" t="s">
+        <v>89</v>
+      </c>
+      <c r="D64" t="s">
+        <v>90</v>
+      </c>
+      <c r="F64" t="s">
+        <v>78</v>
+      </c>
+      <c r="G64" t="s">
+        <v>80</v>
+      </c>
+      <c r="I64" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D65" t="s">
+        <v>101</v>
+      </c>
+      <c r="F65" t="s">
+        <v>78</v>
+      </c>
+      <c r="G65" t="s">
+        <v>80</v>
+      </c>
+      <c r="I65" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" t="s">
+        <v>104</v>
+      </c>
+      <c r="D66" t="s">
+        <v>79</v>
+      </c>
+      <c r="F66" t="s">
+        <v>78</v>
+      </c>
+      <c r="G66" t="s">
+        <v>80</v>
+      </c>
+      <c r="I66" t="s">
         <v>108</v>
       </c>
-      <c r="C64" t="s">
-        <v>105</v>
-      </c>
-      <c r="D64" t="s">
-        <v>80</v>
-      </c>
-      <c r="F64" t="s">
-        <v>79</v>
-      </c>
-      <c r="G64" t="s">
-        <v>81</v>
-      </c>
-      <c r="I64" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B66" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="C66" s="57" t="s">
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B68" s="53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="D68" s="53" t="s">
         <v>133</v>
-      </c>
-      <c r="D66" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="I66" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>102</v>
-      </c>
-      <c r="C67" t="s">
-        <v>92</v>
-      </c>
-      <c r="D67" t="s">
-        <v>105</v>
-      </c>
-      <c r="F67" t="s">
-        <v>121</v>
-      </c>
-      <c r="G67" t="s">
-        <v>107</v>
-      </c>
-      <c r="I67" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" t="s">
-        <v>92</v>
-      </c>
-      <c r="D68" t="s">
-        <v>105</v>
-      </c>
-      <c r="F68" t="s">
-        <v>121</v>
-      </c>
-      <c r="G68" t="s">
-        <v>107</v>
       </c>
       <c r="I68" t="s">
         <v>114</v>
@@ -3268,162 +3253,208 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I69" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I70" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C71" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D71" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I71" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C72" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="D72" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I72" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B76" t="s">
+        <v>111</v>
+      </c>
+      <c r="C73" t="s">
+        <v>83</v>
+      </c>
+      <c r="D73" t="s">
+        <v>104</v>
+      </c>
+      <c r="F73" t="s">
+        <v>120</v>
+      </c>
+      <c r="G73" t="s">
+        <v>106</v>
+      </c>
+      <c r="I73" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" t="s">
+        <v>83</v>
+      </c>
+      <c r="D74" t="s">
+        <v>104</v>
+      </c>
+      <c r="F74" t="s">
+        <v>120</v>
+      </c>
+      <c r="G74" t="s">
+        <v>106</v>
+      </c>
+      <c r="I74" t="s">
         <v>112</v>
       </c>
-      <c r="C76" t="s">
-        <v>83</v>
-      </c>
-      <c r="D76" t="s">
-        <v>84</v>
-      </c>
-      <c r="I76" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>74</v>
-      </c>
-      <c r="B77" t="s">
-        <v>112</v>
-      </c>
-      <c r="C77" t="s">
-        <v>83</v>
-      </c>
-      <c r="D77" t="s">
-        <v>105</v>
-      </c>
-      <c r="E77" t="s">
-        <v>84</v>
-      </c>
-      <c r="I77" t="s">
-        <v>126</v>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B78" t="s">
+        <v>111</v>
+      </c>
+      <c r="C78" t="s">
+        <v>82</v>
+      </c>
+      <c r="D78" t="s">
+        <v>83</v>
+      </c>
+      <c r="I78" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>73</v>
+      </c>
+      <c r="B79" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" t="s">
+        <v>82</v>
+      </c>
+      <c r="D79" t="s">
+        <v>104</v>
+      </c>
+      <c r="E79" t="s">
+        <v>83</v>
+      </c>
+      <c r="I79" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>74</v>
+      </c>
+      <c r="B80" t="s">
+        <v>122</v>
+      </c>
+      <c r="C80" t="s">
         <v>123</v>
       </c>
-      <c r="C78" t="s">
-        <v>124</v>
-      </c>
-      <c r="D78" t="s">
-        <v>103</v>
-      </c>
-      <c r="F78" t="s">
-        <v>130</v>
-      </c>
-      <c r="G78" t="s">
+      <c r="D80" t="s">
+        <v>102</v>
+      </c>
+      <c r="F80" t="s">
         <v>129</v>
       </c>
-      <c r="I78" t="s">
-        <v>122</v>
+      <c r="G80" t="s">
+        <v>128</v>
+      </c>
+      <c r="I80" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3475,7 +3506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5590FB0-7861-4C68-9F7C-2BB835CA7538}">
   <dimension ref="B1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -3489,159 +3520,159 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="64"/>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="59">
+      <c r="B3" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="55">
         <f>20*12*4</f>
         <v>960</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" t="s">
         <v>149</v>
       </c>
-      <c r="D4" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="57">
         <f>POWER($D$3,1 + B5 *0.1)</f>
         <v>960</v>
       </c>
-      <c r="D5" s="63">
+      <c r="D5" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="3">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="65">
+      <c r="C6" s="57">
         <f t="shared" ref="C6:C14" si="0">POWER($D$3,1 + B6 *0.15)</f>
         <v>7532.7335020499258</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>6.2772779183749376</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="3">
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="57">
         <f t="shared" si="0"/>
         <v>59106.327096776331</v>
       </c>
-      <c r="D7" s="63">
+      <c r="D7" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>49.255272580646945</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="3">
+      <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="65">
+      <c r="C8" s="57">
         <f t="shared" si="0"/>
         <v>463783.55240104912</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>386.48629366754091</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="3">
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="65">
+      <c r="C9" s="57">
         <f t="shared" si="0"/>
         <v>3639122.8154907427</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>3032.6023462422859</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="3">
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" s="65">
+      <c r="C10" s="57">
         <f t="shared" si="0"/>
         <v>10193830.257075245</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>8494.8585475627042</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="3">
+      <c r="B11">
         <v>19</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="57">
         <f t="shared" si="0"/>
         <v>303210507415.43286</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>252675422.84619406</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="3">
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="57">
         <f t="shared" si="0"/>
         <v>79986881.970500872</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>66655.734975417392</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="67">
+      <c r="B13" s="59">
         <v>12</v>
       </c>
-      <c r="C13" s="68">
+      <c r="C13" s="60">
         <f t="shared" si="0"/>
         <v>224057482.78930962</v>
       </c>
-      <c r="D13" s="69">
+      <c r="D13" s="61">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>186714.56899109136</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="67">
+      <c r="B14" s="59">
         <v>15</v>
       </c>
-      <c r="C14" s="68">
+      <c r="C14" s="60">
         <f t="shared" si="0"/>
         <v>4924719592.9163141</v>
       </c>
-      <c r="D14" s="69">
+      <c r="D14" s="61">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>4103932.9940969283</v>
       </c>

</xml_diff>

<commit_message>
sawblade holly cider & liquor
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Eigene Dateien\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC870EB-0CEF-4FEA-A028-C60B83501036}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4CC7E7-9815-4D6E-8A7E-EBB74420791F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38370" windowHeight="11670" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
+    <workbookView xWindow="16710" yWindow="0" windowWidth="34890" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Infused Beverages" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="169">
   <si>
     <t>thickness</t>
   </si>
@@ -518,6 +518,21 @@
   </si>
   <si>
     <t>glass_peach_cider</t>
+  </si>
+  <si>
+    <t>sawblade_holly_berry_liquor</t>
+  </si>
+  <si>
+    <t>sawblade_holly_berry_cider</t>
+  </si>
+  <si>
+    <t>sawblade_holly_berry, sugar</t>
+  </si>
+  <si>
+    <t>sawblade_holly_berry</t>
+  </si>
+  <si>
+    <t>projectile_rebound</t>
   </si>
 </sst>
 </file>
@@ -1423,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B33BBD-CB27-4534-9864-9F1639537D70}">
-  <dimension ref="A1:Y85"/>
+  <dimension ref="A1:Y87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2931,7 +2946,7 @@
         <v>163</v>
       </c>
       <c r="B52" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="C52" t="s">
         <v>89</v>
@@ -2954,6 +2969,24 @@
       <c r="Y52" s="54"/>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>165</v>
+      </c>
+      <c r="B53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" t="s">
+        <v>89</v>
+      </c>
+      <c r="F53" t="s">
+        <v>119</v>
+      </c>
+      <c r="G53" t="s">
+        <v>76</v>
+      </c>
+      <c r="I53" t="s">
+        <v>167</v>
+      </c>
       <c r="S53" s="54"/>
       <c r="T53" s="54"/>
       <c r="U53" s="54"/>
@@ -2963,9 +2996,6 @@
       <c r="Y53" s="54"/>
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I54" t="s">
-        <v>115</v>
-      </c>
       <c r="S54" s="54"/>
       <c r="T54" s="54"/>
       <c r="U54" s="54"/>
@@ -2975,23 +3005,8 @@
       <c r="Y54" s="54"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>125</v>
-      </c>
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" t="s">
-        <v>88</v>
-      </c>
-      <c r="F55" t="s">
-        <v>77</v>
-      </c>
-      <c r="G55" t="s">
-        <v>76</v>
-      </c>
       <c r="I55" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="S55" s="54"/>
       <c r="T55" s="54"/>
@@ -3003,10 +3018,10 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C56" t="s">
         <v>88</v>
@@ -3018,7 +3033,7 @@
         <v>76</v>
       </c>
       <c r="I56" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="S56" s="54"/>
       <c r="T56" s="54"/>
@@ -3030,17 +3045,14 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
         <v>88</v>
       </c>
-      <c r="D57" t="s">
-        <v>91</v>
-      </c>
       <c r="F57" t="s">
         <v>77</v>
       </c>
@@ -3048,7 +3060,7 @@
         <v>76</v>
       </c>
       <c r="I57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S57" s="54"/>
       <c r="T57" s="54"/>
@@ -3060,14 +3072,17 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C58" t="s">
         <v>88</v>
       </c>
+      <c r="D58" t="s">
+        <v>91</v>
+      </c>
       <c r="F58" t="s">
         <v>77</v>
       </c>
@@ -3075,7 +3090,7 @@
         <v>76</v>
       </c>
       <c r="I58" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="S58" s="54"/>
       <c r="T58" s="54"/>
@@ -3087,10 +3102,10 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
         <v>88</v>
@@ -3102,7 +3117,7 @@
         <v>76</v>
       </c>
       <c r="I59" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="S59" s="54"/>
       <c r="T59" s="54"/>
@@ -3113,6 +3128,24 @@
       <c r="Y59" s="54"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>159</v>
+      </c>
+      <c r="B60" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" t="s">
+        <v>88</v>
+      </c>
+      <c r="F60" t="s">
+        <v>77</v>
+      </c>
+      <c r="G60" t="s">
+        <v>76</v>
+      </c>
+      <c r="I60" t="s">
+        <v>161</v>
+      </c>
       <c r="S60" s="54"/>
       <c r="T60" s="54"/>
       <c r="U60" s="54"/>
@@ -3122,6 +3155,24 @@
       <c r="Y60" s="54"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" t="s">
+        <v>154</v>
+      </c>
+      <c r="C61" t="s">
+        <v>88</v>
+      </c>
+      <c r="F61" t="s">
+        <v>77</v>
+      </c>
+      <c r="G61" t="s">
+        <v>76</v>
+      </c>
+      <c r="I61" t="s">
+        <v>166</v>
+      </c>
       <c r="S61" s="54"/>
       <c r="T61" s="54"/>
       <c r="U61" s="54"/>
@@ -3131,27 +3182,6 @@
       <c r="Y61" s="54"/>
     </row>
     <row r="62" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>151</v>
-      </c>
-      <c r="B62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" t="s">
-        <v>152</v>
-      </c>
-      <c r="D62" t="s">
-        <v>82</v>
-      </c>
-      <c r="F62" t="s">
-        <v>77</v>
-      </c>
-      <c r="G62" t="s">
-        <v>79</v>
-      </c>
-      <c r="I62" t="s">
-        <v>153</v>
-      </c>
       <c r="S62" s="54"/>
       <c r="T62" s="54"/>
       <c r="U62" s="54"/>
@@ -3161,40 +3191,26 @@
       <c r="Y62" s="54"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>58</v>
-      </c>
-      <c r="B63" t="s">
-        <v>74</v>
-      </c>
-      <c r="C63" t="s">
-        <v>75</v>
-      </c>
-      <c r="D63" t="s">
-        <v>103</v>
-      </c>
-      <c r="F63" t="s">
-        <v>77</v>
-      </c>
-      <c r="G63" t="s">
-        <v>79</v>
-      </c>
-      <c r="I63" t="s">
-        <v>130</v>
-      </c>
+      <c r="S63" s="54"/>
+      <c r="T63" s="54"/>
+      <c r="U63" s="54"/>
+      <c r="V63" s="54"/>
+      <c r="W63" s="54"/>
+      <c r="X63" s="54"/>
+      <c r="Y63" s="54"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C64" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="D64" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F64" t="s">
         <v>77</v>
@@ -3203,21 +3219,28 @@
         <v>79</v>
       </c>
       <c r="I64" t="s">
-        <v>97</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="S64" s="54"/>
+      <c r="T64" s="54"/>
+      <c r="U64" s="54"/>
+      <c r="V64" s="54"/>
+      <c r="W64" s="54"/>
+      <c r="X64" s="54"/>
+      <c r="Y64" s="54"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B65" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C65" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D65" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="F65" t="s">
         <v>77</v>
@@ -3226,21 +3249,21 @@
         <v>79</v>
       </c>
       <c r="I65" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C66" t="s">
         <v>88</v>
       </c>
       <c r="D66" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="F66" t="s">
         <v>77</v>
@@ -3249,21 +3272,21 @@
         <v>79</v>
       </c>
       <c r="I66" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>144</v>
+        <v>60</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C67" t="s">
         <v>88</v>
       </c>
       <c r="D67" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="F67" t="s">
         <v>77</v>
@@ -3272,21 +3295,21 @@
         <v>79</v>
       </c>
       <c r="I67" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="C68" t="s">
         <v>88</v>
       </c>
       <c r="D68" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F68" t="s">
         <v>77</v>
@@ -3295,21 +3318,21 @@
         <v>79</v>
       </c>
       <c r="I68" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
       <c r="B69" t="s">
         <v>106</v>
       </c>
       <c r="C69" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D69" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="F69" t="s">
         <v>77</v>
@@ -3318,75 +3341,75 @@
         <v>79</v>
       </c>
       <c r="I69" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" t="s">
+        <v>88</v>
+      </c>
+      <c r="D70" t="s">
+        <v>100</v>
+      </c>
+      <c r="F70" t="s">
+        <v>77</v>
+      </c>
+      <c r="G70" t="s">
+        <v>79</v>
+      </c>
+      <c r="I70" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" t="s">
+        <v>103</v>
+      </c>
+      <c r="D71" t="s">
+        <v>78</v>
+      </c>
+      <c r="F71" t="s">
+        <v>77</v>
+      </c>
+      <c r="G71" t="s">
+        <v>79</v>
+      </c>
+      <c r="I71" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B72" s="53" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B74" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="C72" s="53" t="s">
+      <c r="C74" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="D72" s="53" t="s">
+      <c r="D74" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I74" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>64</v>
-      </c>
-      <c r="B73" t="s">
-        <v>100</v>
-      </c>
-      <c r="C73" t="s">
-        <v>90</v>
-      </c>
-      <c r="D73" t="s">
-        <v>103</v>
-      </c>
-      <c r="F73" t="s">
-        <v>119</v>
-      </c>
-      <c r="G73" t="s">
-        <v>105</v>
-      </c>
-      <c r="I73" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>67</v>
-      </c>
-      <c r="B74" t="s">
-        <v>89</v>
-      </c>
-      <c r="C74" t="s">
-        <v>90</v>
-      </c>
-      <c r="D74" t="s">
-        <v>103</v>
-      </c>
-      <c r="F74" t="s">
-        <v>119</v>
-      </c>
-      <c r="G74" t="s">
-        <v>105</v>
-      </c>
-      <c r="I74" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B75" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C75" t="s">
         <v>90</v>
@@ -3401,15 +3424,15 @@
         <v>105</v>
       </c>
       <c r="I75" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B76" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C76" t="s">
         <v>90</v>
@@ -3424,18 +3447,18 @@
         <v>105</v>
       </c>
       <c r="I76" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B77" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="C77" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D77" t="s">
         <v>103</v>
@@ -3447,18 +3470,18 @@
         <v>105</v>
       </c>
       <c r="I77" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B78" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" t="s">
         <v>90</v>
-      </c>
-      <c r="C78" t="s">
-        <v>82</v>
       </c>
       <c r="D78" t="s">
         <v>103</v>
@@ -3470,29 +3493,44 @@
         <v>105</v>
       </c>
       <c r="I78" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>110</v>
+      </c>
+      <c r="C79" t="s">
+        <v>82</v>
+      </c>
+      <c r="D79" t="s">
+        <v>103</v>
+      </c>
+      <c r="F79" t="s">
+        <v>119</v>
+      </c>
+      <c r="G79" t="s">
+        <v>105</v>
+      </c>
+      <c r="I79" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>155</v>
+        <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C80" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D80" t="s">
-        <v>154</v>
+        <v>103</v>
       </c>
       <c r="F80" t="s">
         <v>119</v>
@@ -3501,66 +3539,97 @@
         <v>105</v>
       </c>
       <c r="I80" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82" t="s">
+        <v>88</v>
+      </c>
+      <c r="C82" t="s">
+        <v>78</v>
+      </c>
+      <c r="D82" t="s">
+        <v>154</v>
+      </c>
+      <c r="F82" t="s">
+        <v>119</v>
+      </c>
+      <c r="G82" t="s">
+        <v>105</v>
+      </c>
+      <c r="I82" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>71</v>
-      </c>
-      <c r="B83" t="s">
-        <v>110</v>
-      </c>
-      <c r="C83" t="s">
-        <v>81</v>
-      </c>
-      <c r="D83" t="s">
-        <v>82</v>
-      </c>
-      <c r="I83" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>72</v>
-      </c>
-      <c r="B84" t="s">
-        <v>110</v>
-      </c>
-      <c r="C84" t="s">
-        <v>81</v>
-      </c>
-      <c r="D84" t="s">
-        <v>103</v>
-      </c>
-      <c r="E84" t="s">
-        <v>82</v>
-      </c>
-      <c r="I84" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>71</v>
+      </c>
+      <c r="B85" t="s">
+        <v>110</v>
+      </c>
+      <c r="C85" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" t="s">
+        <v>82</v>
+      </c>
+      <c r="I85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>72</v>
+      </c>
+      <c r="B86" t="s">
+        <v>110</v>
+      </c>
+      <c r="C86" t="s">
+        <v>81</v>
+      </c>
+      <c r="D86" t="s">
+        <v>103</v>
+      </c>
+      <c r="E86" t="s">
+        <v>82</v>
+      </c>
+      <c r="I86" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>73</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>121</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C87" t="s">
         <v>122</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D87" t="s">
         <v>101</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F87" t="s">
         <v>128</v>
       </c>
-      <c r="G85" t="s">
+      <c r="G87" t="s">
         <v>127</v>
       </c>
-      <c r="I85" t="s">
+      <c r="I87" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved fermentation logic to an interface
</commit_message>
<xml_diff>
--- a/raw/beverage_calculation.xlsx
+++ b/raw/beverage_calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\FabricModding\Spectrum\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4CC7E7-9815-4D6E-8A7E-EBB74420791F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD23116-A396-4D76-A85D-292A5C8C2738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="0" windowWidth="34890" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34395" windowHeight="21000" xr2:uid="{741EC0C8-7459-47EF-96B2-A8D7740659E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Infused Beverages" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="170">
   <si>
     <t>thickness</t>
   </si>
@@ -533,6 +533,9 @@
   </si>
   <si>
     <t>projectile_rebound</t>
+  </si>
+  <si>
+    <t>days aged (irl days)</t>
   </si>
 </sst>
 </file>
@@ -654,7 +657,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -919,13 +922,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -936,11 +965,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -957,7 +982,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1005,6 +1029,14 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
@@ -1094,31 +1126,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}" name="Tabelle1" displayName="Tabelle1" ref="A20:I39" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A20:I39" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}" name="Tabelle1" displayName="Tabelle1" ref="A21:I40" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A21:I40" xr:uid="{C236F747-143F-4A20-AE07-A5D51D9E199B}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{01EC8C57-83BE-4610-A43F-E9C497C3103A}" name="Beverage Type" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{3AFBF746-223D-4849-8D15-6B5EBC41CD07}" name="Ferm.Mod" dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{1E074399-223F-4717-8110-138418658072}" name="32">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B22)/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{22C31000-51B9-4B7F-B422-644C6EF1B656}" name="72">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B22)/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{8E06E958-7DE2-473E-B292-951C29C62EF1}" name="144">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B22)/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{B74AAB8D-B30F-46F4-A6AE-682A6EAB9131}" name="216">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B22)/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{C2DF63A0-3F23-448A-B439-244AD8443B28}" name="288">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B22)/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{253E0318-1896-406A-A446-939D5EA3C3B1}" name="1008">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B22)/100)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{1D17B4C3-392F-435C-82A2-4BFC2C15EC49}" name="2160" dataDxfId="3">
-      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B21)/100)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B22)/100)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1438,10 +1470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B33BBD-CB27-4534-9864-9F1639537D70}">
-  <dimension ref="A1:Y87"/>
+  <dimension ref="A1:Y88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I61" sqref="I61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1463,7 +1495,7 @@
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="22">
         <v>18</v>
       </c>
       <c r="D3" t="s">
@@ -1474,8 +1506,8 @@
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="27">
-        <v>2</v>
+      <c r="B4" s="23">
+        <v>1</v>
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
@@ -1526,40 +1558,40 @@
       <c r="A7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="24">
         <v>18</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="16">
         <v>18</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="16">
         <v>18</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="16">
         <v>18</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="16">
         <v>18</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="16">
         <v>18</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="16">
         <v>18</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="16">
         <v>18</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="16">
         <v>18</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7" s="16">
         <v>18</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="16">
         <v>18</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="17">
         <v>18</v>
       </c>
       <c r="O7" t="s">
@@ -1570,40 +1602,40 @@
       <c r="A8" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="25">
+        <v>24</v>
+      </c>
+      <c r="C8" s="18">
         <v>72</v>
       </c>
-      <c r="C8" s="22">
-        <v>144</v>
-      </c>
-      <c r="D8" s="22">
-        <v>196</v>
-      </c>
-      <c r="E8" s="22">
-        <v>196</v>
-      </c>
-      <c r="F8" s="22">
-        <v>196</v>
-      </c>
-      <c r="G8" s="22">
+      <c r="D8" s="18">
+        <v>240</v>
+      </c>
+      <c r="E8" s="18">
+        <v>240</v>
+      </c>
+      <c r="F8" s="18">
+        <v>240</v>
+      </c>
+      <c r="G8" s="18">
         <v>72</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="18">
         <v>72</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="18">
         <v>72</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="18">
         <v>72</v>
       </c>
-      <c r="K8" s="22">
+      <c r="K8" s="18">
         <v>72</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="18">
         <v>72</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="19">
         <v>72</v>
       </c>
       <c r="O8" t="s">
@@ -1614,40 +1646,40 @@
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="26">
         <v>0.4</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="20">
         <v>0.4</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="20">
         <v>0.4</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="20">
         <v>1</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="20">
         <v>0</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="20">
         <v>0.4</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="20">
         <v>0.4</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="20">
         <v>0.4</v>
       </c>
-      <c r="J9" s="24">
+      <c r="J9" s="20">
         <v>0.4</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K9" s="20">
         <v>0.4</v>
       </c>
-      <c r="L9" s="24">
+      <c r="L9" s="20">
         <v>0.4</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="21">
         <v>0.4</v>
       </c>
       <c r="O9" t="s">
@@ -1685,56 +1717,56 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="65">
         <f>B8*3</f>
+        <v>72</v>
+      </c>
+      <c r="C12" s="66">
+        <f>C8*3</f>
         <v>216</v>
       </c>
-      <c r="C12" s="13">
-        <f t="shared" ref="C12:M12" si="0">C8*3</f>
-        <v>432</v>
-      </c>
-      <c r="D12" s="13">
-        <f t="shared" si="0"/>
-        <v>588</v>
-      </c>
-      <c r="E12" s="13">
-        <f t="shared" si="0"/>
-        <v>588</v>
-      </c>
-      <c r="F12" s="13">
-        <f t="shared" si="0"/>
-        <v>588</v>
-      </c>
-      <c r="G12" s="13">
-        <f t="shared" si="0"/>
+      <c r="D12" s="66">
+        <f>D8*3</f>
+        <v>720</v>
+      </c>
+      <c r="E12" s="66">
+        <f>E8*3</f>
+        <v>720</v>
+      </c>
+      <c r="F12" s="66">
+        <f>F8*3</f>
+        <v>720</v>
+      </c>
+      <c r="G12" s="66">
+        <f>G8*3</f>
         <v>216</v>
       </c>
-      <c r="H12" s="13">
-        <f t="shared" si="0"/>
+      <c r="H12" s="66">
+        <f>H8*3</f>
         <v>216</v>
       </c>
-      <c r="I12" s="13">
-        <f t="shared" si="0"/>
+      <c r="I12" s="66">
+        <f>I8*3</f>
         <v>216</v>
       </c>
-      <c r="J12" s="13">
-        <f t="shared" si="0"/>
+      <c r="J12" s="66">
+        <f>J8*3</f>
         <v>216</v>
       </c>
-      <c r="K12" s="13">
-        <f t="shared" si="0"/>
+      <c r="K12" s="66">
+        <f>K8*3</f>
         <v>216</v>
       </c>
-      <c r="L12" s="13">
-        <f t="shared" si="0"/>
+      <c r="L12" s="66">
+        <f>L8*3</f>
         <v>216</v>
       </c>
-      <c r="M12" s="14">
-        <f t="shared" si="0"/>
+      <c r="M12" s="67">
+        <f>M8*3</f>
         <v>216</v>
       </c>
       <c r="O12" t="s">
@@ -1742,734 +1774,748 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="60">
+        <f>B12/72</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="60">
+        <f t="shared" ref="C13:M13" si="0">C12/72</f>
+        <v>3</v>
+      </c>
+      <c r="D13" s="60">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E13" s="60">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F13" s="60">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G13" s="60">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H13" s="60">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I13" s="60">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J13" s="60">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K13" s="60">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L13" s="60">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M13" s="61">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B14" s="27">
         <f>B7/$B$3</f>
         <v>1</v>
       </c>
-      <c r="C13" s="15">
-        <f t="shared" ref="C13:M13" si="1">C7/$B$3</f>
+      <c r="C14" s="11">
+        <f>C7/$B$3</f>
         <v>1</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D14" s="11">
+        <f>D7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
+        <f>E7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="11">
+        <f>F7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="11">
+        <f>G7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="11">
+        <f>H7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="11">
+        <f>I7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="11">
+        <f>J7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="11">
+        <f>K7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="L14" s="11">
+        <f>L7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="M14" s="12">
+        <f>M7/$B$3</f>
+        <v>1</v>
+      </c>
+      <c r="O14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="28">
+        <f>IF($B$4=0,0,LOG(B12*(0.5+B14/2)*(0.5+B9/2),1+$B$4)/100)</f>
+        <v>5.6553518286125544E-2</v>
+      </c>
+      <c r="C15" s="13">
+        <f>IF($B$4=0,0,LOG(C12*(0.5+C14/2)*(0.5+C9/2),1+$B$4)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="D15" s="13">
+        <f>IF($B$4=0,0,LOG(D12*(0.5+D14/2)*(0.5+D9/2),1+$B$4)/100)</f>
+        <v>8.9772799234999173E-2</v>
+      </c>
+      <c r="E15" s="13">
+        <f>IF($B$4=0,0,LOG(E12*(0.5+E14/2)*(0.5+E9/2),1+$B$4)/100)</f>
+        <v>9.4918530963296763E-2</v>
+      </c>
+      <c r="F15" s="13">
+        <f>IF($B$4=0,0,LOG(F12*(0.5+F14/2)*(0.5+F9/2),1+$B$4)/100)</f>
+        <v>8.4918530963296754E-2</v>
+      </c>
+      <c r="G15" s="13">
+        <f>IF($B$4=0,0,LOG(G12*(0.5+G14/2)*(0.5+G9/2),1+$B$4)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="H15" s="13">
+        <f>IF($B$4=0,0,LOG(H12*(0.5+H14/2)*(0.5+H9/2),1+$B$4)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="I15" s="13">
+        <f>IF($B$4=0,0,LOG(I12*(0.5+I14/2)*(0.5+I9/2),1+$B$4)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="J15" s="13">
+        <f>IF($B$4=0,0,LOG(J12*(0.5+J14/2)*(0.5+J9/2),1+$B$4)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="K15" s="13">
+        <f>IF($B$4=0,0,LOG(K12*(0.5+K14/2)*(0.5+K9/2),1+$B$4)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="L15" s="13">
+        <f>IF($B$4=0,0,LOG(L12*(0.5+L14/2)*(0.5+L9/2),1+$B$4)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="M15" s="14">
+        <f>IF($B$4=0,0,LOG(M12*(0.5+M14/2)*(0.5+M9/2),1+$B$4)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="O15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15">
+        <f>ABS(1.5-B14/2)</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="15">
+        <f>ABS(1.5-C14/2)</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="15">
+        <f t="shared" ref="D16:M16" si="1">ABS(1.5-D14/2)</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E13" s="15">
+      <c r="F16" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F13" s="15">
+      <c r="G16" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G13" s="15">
+      <c r="H16" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="H13" s="15">
+      <c r="I16" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I13" s="15">
+      <c r="J16" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J13" s="15">
+      <c r="K16" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K13" s="15">
+      <c r="L16" s="15">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L13" s="15">
+      <c r="M16" s="63">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M13" s="16">
-        <f t="shared" si="1"/>
+      <c r="O16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="36">
         <v>1</v>
       </c>
-      <c r="O13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="33">
-        <f>IF($B$4=0,0,LOG(B12*(0.5+B13/2)*(0.5+B9/2),1+$B$4)/100)</f>
-        <v>4.5681297355864098E-2</v>
-      </c>
-      <c r="C14" s="17">
-        <f t="shared" ref="C14:M14" si="2">IF($B$4=0,0,LOG(C12*(0.5+C13/2)*(0.5+C9/2),1+$B$4)/100)</f>
-        <v>5.1990594891578673E-2</v>
-      </c>
-      <c r="D14" s="17">
-        <f t="shared" si="2"/>
-        <v>5.4796874803377964E-2</v>
-      </c>
-      <c r="E14" s="17">
-        <f t="shared" si="2"/>
-        <v>5.8043470054657584E-2</v>
-      </c>
-      <c r="F14" s="17">
-        <f t="shared" si="2"/>
-        <v>5.1734172518943015E-2</v>
-      </c>
-      <c r="G14" s="17">
-        <f t="shared" si="2"/>
-        <v>4.5681297355864098E-2</v>
-      </c>
-      <c r="H14" s="17">
-        <f t="shared" si="2"/>
-        <v>4.5681297355864098E-2</v>
-      </c>
-      <c r="I14" s="17">
-        <f t="shared" si="2"/>
-        <v>4.5681297355864098E-2</v>
-      </c>
-      <c r="J14" s="17">
-        <f t="shared" si="2"/>
-        <v>4.5681297355864098E-2</v>
-      </c>
-      <c r="K14" s="17">
-        <f t="shared" si="2"/>
-        <v>4.5681297355864098E-2</v>
-      </c>
-      <c r="L14" s="17">
-        <f t="shared" si="2"/>
-        <v>4.5681297355864098E-2</v>
-      </c>
-      <c r="M14" s="18">
-        <f t="shared" si="2"/>
-        <v>4.5681297355864098E-2</v>
-      </c>
-      <c r="O14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="19">
-        <f>ABS(1.5-B13/2)</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="19">
-        <f>ABS(1.5-C13/2)</f>
-        <v>1</v>
-      </c>
-      <c r="D15" s="19">
-        <f t="shared" ref="D15:M15" si="3">ABS(1.5-D13/2)</f>
-        <v>1</v>
-      </c>
-      <c r="E15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="F15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="G15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="H15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="J15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="K15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M15" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="O15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="41">
-        <v>1</v>
-      </c>
-      <c r="G18" s="39" t="s">
+      <c r="G19" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H18" s="41">
+      <c r="H19" s="36">
         <v>0.4</v>
       </c>
-      <c r="I18" s="40"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="42"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43" t="s">
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D20" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E20" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F20" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="43" t="s">
+      <c r="G20" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="43" t="s">
+      <c r="H20" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="44" t="s">
+      <c r="I20" s="39" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>44</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>138</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>32</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>137</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F21" t="s">
         <v>136</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>139</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>140</v>
       </c>
-      <c r="I20" s="35" t="s">
+      <c r="I21" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K21" t="s">
         <v>45</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="34" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="50">
+      <c r="B22" s="45">
         <v>0</v>
       </c>
-      <c r="C21" s="48">
+      <c r="C22" s="43">
         <v>0</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D22" s="43">
         <v>0</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E22" s="43">
         <v>0</v>
       </c>
-      <c r="F21" s="48">
+      <c r="F22" s="43">
         <v>0</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G22" s="43">
         <v>0</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H22" s="43">
         <v>0</v>
       </c>
-      <c r="I21" s="49">
+      <c r="I22" s="44">
         <v>0</v>
-      </c>
-      <c r="K21">
-        <v>4</v>
-      </c>
-      <c r="L21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="51">
-        <v>1.25</v>
-      </c>
-      <c r="C22" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>3.833943903789129E-2</v>
-      </c>
-      <c r="D22" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>4.8339439037891292E-2</v>
-      </c>
-      <c r="E22" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>5.6886995494648568E-2</v>
-      </c>
-      <c r="F22" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>6.1886995494648572E-2</v>
-      </c>
-      <c r="G22" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>6.543455195140585E-2</v>
-      </c>
-      <c r="H22" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>8.0883020185091359E-2</v>
-      </c>
-      <c r="I22" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B22)/100)</f>
-        <v>9.028136343098643E-2</v>
       </c>
       <c r="K22">
         <v>4</v>
       </c>
       <c r="L22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="51">
+        <v>21</v>
+      </c>
+      <c r="B23" s="46">
         <v>1.25</v>
       </c>
-      <c r="C23" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+      <c r="C23" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B23)/100)</f>
         <v>3.833943903789129E-2</v>
       </c>
-      <c r="D23" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+      <c r="D23" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B23)/100)</f>
         <v>4.8339439037891292E-2</v>
       </c>
-      <c r="E23" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+      <c r="E23" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B23)/100)</f>
         <v>5.6886995494648568E-2</v>
       </c>
-      <c r="F23" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+      <c r="F23" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B23)/100)</f>
         <v>6.1886995494648572E-2</v>
       </c>
-      <c r="G23" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+      <c r="G23" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B23)/100)</f>
         <v>6.543455195140585E-2</v>
       </c>
-      <c r="H23" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+      <c r="H23" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B23)/100)</f>
         <v>8.0883020185091359E-2</v>
       </c>
-      <c r="I23" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B23)/100)</f>
+      <c r="I23" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B23)/100)</f>
         <v>9.028136343098643E-2</v>
       </c>
       <c r="K23">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="L23" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="51">
-        <v>0.25</v>
-      </c>
-      <c r="C24" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.13933008328271637</v>
-      </c>
-      <c r="D24" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.17567127313294212</v>
-      </c>
-      <c r="E24" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.20673411032799602</v>
-      </c>
-      <c r="F24" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.22490470525310891</v>
-      </c>
-      <c r="G24" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.23779694752304992</v>
-      </c>
-      <c r="H24" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.2939385192206046</v>
-      </c>
-      <c r="I24" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B24)/100)</f>
-        <v>0.32809321683827058</v>
+        <v>35</v>
+      </c>
+      <c r="B24" s="46">
+        <v>1.25</v>
+      </c>
+      <c r="C24" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B24)/100)</f>
+        <v>3.833943903789129E-2</v>
+      </c>
+      <c r="D24" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B24)/100)</f>
+        <v>4.8339439037891292E-2</v>
+      </c>
+      <c r="E24" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B24)/100)</f>
+        <v>5.6886995494648568E-2</v>
+      </c>
+      <c r="F24" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B24)/100)</f>
+        <v>6.1886995494648572E-2</v>
+      </c>
+      <c r="G24" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B24)/100)</f>
+        <v>6.543455195140585E-2</v>
+      </c>
+      <c r="H24" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B24)/100)</f>
+        <v>8.0883020185091359E-2</v>
+      </c>
+      <c r="I24" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B24)/100)</f>
+        <v>9.028136343098643E-2</v>
       </c>
       <c r="K24">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="L24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="51">
-        <v>0.125</v>
-      </c>
-      <c r="C25" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.26396508983953099</v>
-      </c>
-      <c r="D25" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.33281458176314815</v>
-      </c>
-      <c r="E25" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.39166407368676537</v>
-      </c>
-      <c r="F25" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.42608881964857398</v>
-      </c>
-      <c r="G25" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.45051356561038253</v>
-      </c>
-      <c r="H25" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.55687548449912128</v>
-      </c>
-      <c r="I25" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B25)/100)</f>
-        <v>0.62158260023948475</v>
+        <v>37</v>
+      </c>
+      <c r="B25" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="C25" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B25)/100)</f>
+        <v>0.13933008328271637</v>
+      </c>
+      <c r="D25" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B25)/100)</f>
+        <v>0.17567127313294212</v>
+      </c>
+      <c r="E25" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B25)/100)</f>
+        <v>0.20673411032799602</v>
+      </c>
+      <c r="F25" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B25)/100)</f>
+        <v>0.22490470525310891</v>
+      </c>
+      <c r="G25" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B25)/100)</f>
+        <v>0.23779694752304992</v>
+      </c>
+      <c r="H25" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B25)/100)</f>
+        <v>0.2939385192206046</v>
+      </c>
+      <c r="I25" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B25)/100)</f>
+        <v>0.32809321683827058</v>
       </c>
       <c r="K25">
         <v>24</v>
       </c>
       <c r="L25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="46">
+        <v>0.125</v>
+      </c>
+      <c r="C26" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B26)/100)</f>
+        <v>0.26396508983953099</v>
+      </c>
+      <c r="D26" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B26)/100)</f>
+        <v>0.33281458176314815</v>
+      </c>
+      <c r="E26" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B26)/100)</f>
+        <v>0.39166407368676537</v>
+      </c>
+      <c r="F26" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B26)/100)</f>
+        <v>0.42608881964857398</v>
+      </c>
+      <c r="G26" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B26)/100)</f>
+        <v>0.45051356561038253</v>
+      </c>
+      <c r="H26" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B26)/100)</f>
+        <v>0.55687548449912128</v>
+      </c>
+      <c r="I26" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B26)/100)</f>
+        <v>0.62158260023948475</v>
+      </c>
+      <c r="K26">
+        <v>24</v>
+      </c>
+      <c r="L26" t="s">
         <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
-        <v/>
-      </c>
-      <c r="D26" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
-        <v/>
-      </c>
-      <c r="E26" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
-        <v/>
-      </c>
-      <c r="F26" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
-        <v/>
-      </c>
-      <c r="G26" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
-        <v/>
-      </c>
-      <c r="H26" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
-        <v/>
-      </c>
-      <c r="I26" s="37" t="str">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B26)/100)</f>
-        <v/>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
-        <v/>
-      </c>
-      <c r="D27" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
-        <v/>
-      </c>
-      <c r="E27" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
-        <v/>
-      </c>
-      <c r="F27" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
-        <v/>
-      </c>
-      <c r="G27" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
-        <v/>
-      </c>
-      <c r="H27" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
-        <v/>
-      </c>
-      <c r="I27" s="37" t="str">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B27)/100)</f>
+      <c r="B27" s="46"/>
+      <c r="C27" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="D27" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="E27" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="F27" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="G27" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="H27" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B27)/100)</f>
+        <v/>
+      </c>
+      <c r="I27" s="32" t="str">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B27)/100)</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
-        <v/>
-      </c>
-      <c r="D28" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
-        <v/>
-      </c>
-      <c r="E28" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
-        <v/>
-      </c>
-      <c r="F28" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
-        <v/>
-      </c>
-      <c r="G28" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
-        <v/>
-      </c>
-      <c r="H28" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
-        <v/>
-      </c>
-      <c r="I28" s="37" t="str">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B28)/100)</f>
+      <c r="B28" s="46"/>
+      <c r="C28" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="D28" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="E28" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="F28" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="G28" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="H28" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B28)/100)</f>
+        <v/>
+      </c>
+      <c r="I28" s="32" t="str">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B28)/100)</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
-        <v/>
-      </c>
-      <c r="D29" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
-        <v/>
-      </c>
-      <c r="E29" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
-        <v/>
-      </c>
-      <c r="F29" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
-        <v/>
-      </c>
-      <c r="G29" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
-        <v/>
-      </c>
-      <c r="H29" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
-        <v/>
-      </c>
-      <c r="I29" s="37" t="str">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B29)/100)</f>
+      <c r="B29" s="46"/>
+      <c r="C29" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="D29" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="E29" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="F29" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="G29" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="H29" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B29)/100)</f>
+        <v/>
+      </c>
+      <c r="I29" s="32" t="str">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B29)/100)</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
-        <v/>
-      </c>
-      <c r="D30" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
-        <v/>
-      </c>
-      <c r="E30" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
-        <v/>
-      </c>
-      <c r="F30" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
-        <v/>
-      </c>
-      <c r="G30" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
-        <v/>
-      </c>
-      <c r="H30" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
-        <v/>
-      </c>
-      <c r="I30" s="37" t="str">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B30)/100)</f>
+      <c r="B30" s="46"/>
+      <c r="C30" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="D30" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="E30" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="F30" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="G30" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="H30" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B30)/100)</f>
+        <v/>
+      </c>
+      <c r="I30" s="32" t="str">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B30)/100)</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="51">
-        <v>0.1</v>
-      </c>
-      <c r="C31" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.32620450042629268</v>
-      </c>
-      <c r="D31" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.41128777462441041</v>
-      </c>
-      <c r="E31" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.48401318359782758</v>
-      </c>
-      <c r="F31" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.52655482069688653</v>
-      </c>
-      <c r="G31" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.55673859257124469</v>
-      </c>
-      <c r="H31" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.68817921843800245</v>
-      </c>
-      <c r="I31" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B31)/100)</f>
-        <v>0.76814339997785419</v>
-      </c>
-      <c r="K31">
-        <v>48</v>
+      <c r="A31" s="1"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B31)/100)</f>
+        <v/>
+      </c>
+      <c r="D31" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B31)/100)</f>
+        <v/>
+      </c>
+      <c r="E31" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B31)/100)</f>
+        <v/>
+      </c>
+      <c r="F31" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B31)/100)</f>
+        <v/>
+      </c>
+      <c r="G31" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B31)/100)</f>
+        <v/>
+      </c>
+      <c r="H31" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B31)/100)</f>
+        <v/>
+      </c>
+      <c r="I31" s="32" t="str">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B31)/100)</f>
+        <v/>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="51">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C32" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.42989940785288216</v>
-      </c>
-      <c r="D32" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.54202921951444771</v>
-      </c>
-      <c r="E32" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.63787280908072685</v>
-      </c>
-      <c r="F32" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.69393771491150957</v>
-      </c>
-      <c r="G32" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.733716398647006</v>
-      </c>
-      <c r="H32" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>0.90693978199728931</v>
-      </c>
-      <c r="I32" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B32)/100)</f>
-        <v>1.0123232278065855</v>
+        <v>38</v>
+      </c>
+      <c r="B32" s="46">
+        <v>0.1</v>
+      </c>
+      <c r="C32" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B32)/100)</f>
+        <v>0.32620450042629268</v>
+      </c>
+      <c r="D32" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B32)/100)</f>
+        <v>0.41128777462441041</v>
+      </c>
+      <c r="E32" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B32)/100)</f>
+        <v>0.48401318359782758</v>
+      </c>
+      <c r="F32" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B32)/100)</f>
+        <v>0.52655482069688653</v>
+      </c>
+      <c r="G32" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B32)/100)</f>
+        <v>0.55673859257124469</v>
+      </c>
+      <c r="H32" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B32)/100)</f>
+        <v>0.68817921843800245</v>
+      </c>
+      <c r="I32" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B32)/100)</f>
+        <v>0.76814339997785419</v>
       </c>
       <c r="K32">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="51">
-        <v>0.25</v>
-      </c>
-      <c r="C33" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.13933008328271637</v>
-      </c>
-      <c r="D33" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.17567127313294212</v>
-      </c>
-      <c r="E33" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.20673411032799602</v>
-      </c>
-      <c r="F33" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.22490470525310891</v>
-      </c>
-      <c r="G33" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.23779694752304992</v>
-      </c>
-      <c r="H33" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.2939385192206046</v>
-      </c>
-      <c r="I33" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B33)/100)</f>
-        <v>0.32809321683827058</v>
+        <v>39</v>
+      </c>
+      <c r="B33" s="46">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C33" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B33)/100)</f>
+        <v>0.42989940785288216</v>
+      </c>
+      <c r="D33" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B33)/100)</f>
+        <v>0.54202921951444771</v>
+      </c>
+      <c r="E33" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B33)/100)</f>
+        <v>0.63787280908072685</v>
+      </c>
+      <c r="F33" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B33)/100)</f>
+        <v>0.69393771491150957</v>
+      </c>
+      <c r="G33" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B33)/100)</f>
+        <v>0.733716398647006</v>
+      </c>
+      <c r="H33" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B33)/100)</f>
+        <v>0.90693978199728931</v>
+      </c>
+      <c r="I33" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B33)/100)</f>
+        <v>1.0123232278065855</v>
       </c>
       <c r="K33">
         <v>72</v>
@@ -2477,248 +2523,266 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="51">
-        <v>0.5</v>
-      </c>
-      <c r="C34" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>7.6678878075782581E-2</v>
-      </c>
-      <c r="D34" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>9.6678878075782584E-2</v>
-      </c>
-      <c r="E34" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>0.11377399098929714</v>
-      </c>
-      <c r="F34" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>0.12377399098929714</v>
-      </c>
-      <c r="G34" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>0.1308691039028117</v>
-      </c>
-      <c r="H34" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>0.16176604037018272</v>
-      </c>
-      <c r="I34" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B34)/100)</f>
-        <v>0.18056272686197286</v>
+        <v>40</v>
+      </c>
+      <c r="B34" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="C34" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B34)/100)</f>
+        <v>0.13933008328271637</v>
+      </c>
+      <c r="D34" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B34)/100)</f>
+        <v>0.17567127313294212</v>
+      </c>
+      <c r="E34" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B34)/100)</f>
+        <v>0.20673411032799602</v>
+      </c>
+      <c r="F34" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B34)/100)</f>
+        <v>0.22490470525310891</v>
+      </c>
+      <c r="G34" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B34)/100)</f>
+        <v>0.23779694752304992</v>
+      </c>
+      <c r="H34" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B34)/100)</f>
+        <v>0.2939385192206046</v>
+      </c>
+      <c r="I34" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B34)/100)</f>
+        <v>0.32809321683827058</v>
       </c>
       <c r="K34">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="51">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C35" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.42989940785288216</v>
-      </c>
-      <c r="D35" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.54202921951444771</v>
-      </c>
-      <c r="E35" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.63787280908072685</v>
-      </c>
-      <c r="F35" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.69393771491150957</v>
-      </c>
-      <c r="G35" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.733716398647006</v>
-      </c>
-      <c r="H35" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>0.90693978199728931</v>
-      </c>
-      <c r="I35" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B35)/100)</f>
-        <v>1.0123232278065855</v>
+        <v>41</v>
+      </c>
+      <c r="B35" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="C35" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B35)/100)</f>
+        <v>7.6678878075782581E-2</v>
+      </c>
+      <c r="D35" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B35)/100)</f>
+        <v>9.6678878075782584E-2</v>
+      </c>
+      <c r="E35" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B35)/100)</f>
+        <v>0.11377399098929714</v>
+      </c>
+      <c r="F35" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B35)/100)</f>
+        <v>0.12377399098929714</v>
+      </c>
+      <c r="G35" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B35)/100)</f>
+        <v>0.1308691039028117</v>
+      </c>
+      <c r="H35" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B35)/100)</f>
+        <v>0.16176604037018272</v>
+      </c>
+      <c r="I35" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B35)/100)</f>
+        <v>0.18056272686197286</v>
       </c>
       <c r="K35">
         <v>24</v>
       </c>
-      <c r="L35" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="51">
-        <v>1</v>
-      </c>
-      <c r="C36" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>4.485426827170242E-2</v>
-      </c>
-      <c r="D36" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>5.6553518286125544E-2</v>
-      </c>
-      <c r="E36" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>6.6553518286125546E-2</v>
-      </c>
-      <c r="F36" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>7.2403143293337108E-2</v>
-      </c>
-      <c r="G36" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>7.6553518286125541E-2</v>
-      </c>
-      <c r="H36" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>9.4627067506701593E-2</v>
-      </c>
-      <c r="I36" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B36)/100)</f>
-        <v>0.10562242424221072</v>
+        <v>46</v>
+      </c>
+      <c r="B36" s="46">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C36" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B36)/100)</f>
+        <v>0.42989940785288216</v>
+      </c>
+      <c r="D36" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B36)/100)</f>
+        <v>0.54202921951444771</v>
+      </c>
+      <c r="E36" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B36)/100)</f>
+        <v>0.63787280908072685</v>
+      </c>
+      <c r="F36" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B36)/100)</f>
+        <v>0.69393771491150957</v>
+      </c>
+      <c r="G36" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B36)/100)</f>
+        <v>0.733716398647006</v>
+      </c>
+      <c r="H36" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B36)/100)</f>
+        <v>0.90693978199728931</v>
+      </c>
+      <c r="I36" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B36)/100)</f>
+        <v>1.0123232278065855</v>
       </c>
       <c r="K36">
-        <v>4</v>
+        <v>24</v>
+      </c>
+      <c r="L36" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="46">
+        <v>1</v>
+      </c>
+      <c r="C37" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B37)/100)</f>
+        <v>4.485426827170242E-2</v>
+      </c>
+      <c r="D37" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B37)/100)</f>
+        <v>5.6553518286125544E-2</v>
+      </c>
+      <c r="E37" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B37)/100)</f>
+        <v>6.6553518286125546E-2</v>
+      </c>
+      <c r="F37" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B37)/100)</f>
+        <v>7.2403143293337108E-2</v>
+      </c>
+      <c r="G37" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B37)/100)</f>
+        <v>7.6553518286125541E-2</v>
+      </c>
+      <c r="H37" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B37)/100)</f>
+        <v>9.4627067506701593E-2</v>
+      </c>
+      <c r="I37" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B37)/100)</f>
+        <v>0.10562242424221072</v>
+      </c>
+      <c r="K37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="51">
+      <c r="B38" s="46">
         <v>1</v>
       </c>
-      <c r="C37" s="36">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+      <c r="C38" s="31">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B38)/100)</f>
         <v>4.485426827170242E-2</v>
       </c>
-      <c r="D37" s="36">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+      <c r="D38" s="31">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B38)/100)</f>
         <v>5.6553518286125544E-2</v>
       </c>
-      <c r="E37" s="36">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+      <c r="E38" s="31">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B38)/100)</f>
         <v>6.6553518286125546E-2</v>
       </c>
-      <c r="F37" s="36">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+      <c r="F38" s="31">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B38)/100)</f>
         <v>7.2403143293337108E-2</v>
       </c>
-      <c r="G37" s="36">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+      <c r="G38" s="31">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B38)/100)</f>
         <v>7.6553518286125541E-2</v>
       </c>
-      <c r="H37" s="36">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+      <c r="H38" s="31">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B38)/100)</f>
         <v>9.4627067506701593E-2</v>
       </c>
-      <c r="I37" s="37">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B37)/100)</f>
+      <c r="I38" s="32">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B38)/100)</f>
         <v>0.10562242424221072</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="51"/>
-      <c r="C38" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
-        <v/>
-      </c>
-      <c r="D38" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
-        <v/>
-      </c>
-      <c r="E38" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
-        <v/>
-      </c>
-      <c r="F38" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
-        <v/>
-      </c>
-      <c r="G38" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
-        <v/>
-      </c>
-      <c r="H38" s="36" t="str">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
-        <v/>
-      </c>
-      <c r="I38" s="37" t="str">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B38)/100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="38"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="46" t="str">
-        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
-        <v/>
-      </c>
-      <c r="D39" s="46" t="str">
-        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
-        <v/>
-      </c>
-      <c r="E39" s="46" t="str">
-        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
-        <v/>
-      </c>
-      <c r="F39" s="46" t="str">
-        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
-        <v/>
-      </c>
-      <c r="G39" s="46" t="str">
-        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
-        <v/>
-      </c>
-      <c r="H39" s="46" t="str">
-        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
-        <v/>
-      </c>
-      <c r="I39" s="47" t="str">
-        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$20*(0.5+$F$18/2)*(0.5+$H$18/2),1+$B39)/100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" t="s">
-        <v>74</v>
-      </c>
-      <c r="I42" t="s">
-        <v>87</v>
-      </c>
-      <c r="S42" s="54"/>
-      <c r="T42" s="54"/>
-      <c r="U42" s="54"/>
-      <c r="V42" s="54"/>
-      <c r="W42" s="54"/>
-      <c r="X42" s="54"/>
-      <c r="Y42" s="54"/>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="D39" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="E39" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="F39" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="G39" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="H39" s="31" t="str">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+      <c r="I39" s="32" t="str">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B39)/100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="33"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[Ferm.Mod]]="","",LOG(C$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B40)/100)</f>
+        <v/>
+      </c>
+      <c r="D40" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[32]]="","",LOG(D$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B40)/100)</f>
+        <v/>
+      </c>
+      <c r="E40" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[72]]="","",LOG(E$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B40)/100)</f>
+        <v/>
+      </c>
+      <c r="F40" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[144]]="","",LOG(F$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B40)/100)</f>
+        <v/>
+      </c>
+      <c r="G40" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[216]]="","",LOG(G$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B40)/100)</f>
+        <v/>
+      </c>
+      <c r="H40" s="41" t="str">
+        <f>IF(Tabelle1[[#This Row],[288]]="","",LOG(H$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B40)/100)</f>
+        <v/>
+      </c>
+      <c r="I40" s="42" t="str">
+        <f>IF(Tabelle1[[#This Row],[1008]]="","",LOG(I$21*(0.5+$F$19/2)*(0.5+$H$19/2),1+$B40)/100)</f>
+        <v/>
+      </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
         <v>80</v>
@@ -2726,32 +2790,23 @@
       <c r="C43" t="s">
         <v>74</v>
       </c>
-      <c r="D43" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" t="s">
-        <v>129</v>
-      </c>
-      <c r="G43" t="s">
-        <v>76</v>
-      </c>
       <c r="I43" t="s">
-        <v>84</v>
-      </c>
-      <c r="S43" s="54"/>
-      <c r="T43" s="54"/>
-      <c r="U43" s="54"/>
-      <c r="V43" s="54"/>
-      <c r="W43" s="54"/>
-      <c r="X43" s="54"/>
-      <c r="Y43" s="54"/>
+        <v>87</v>
+      </c>
+      <c r="S43" s="49"/>
+      <c r="T43" s="49"/>
+      <c r="U43" s="49"/>
+      <c r="V43" s="49"/>
+      <c r="W43" s="49"/>
+      <c r="X43" s="49"/>
+      <c r="Y43" s="49"/>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
         <v>74</v>
@@ -2766,22 +2821,22 @@
         <v>76</v>
       </c>
       <c r="I44" t="s">
-        <v>83</v>
-      </c>
-      <c r="S44" s="54"/>
-      <c r="T44" s="54"/>
-      <c r="U44" s="54"/>
-      <c r="V44" s="54"/>
-      <c r="W44" s="54"/>
-      <c r="X44" s="54"/>
-      <c r="Y44" s="54"/>
+        <v>84</v>
+      </c>
+      <c r="S44" s="49"/>
+      <c r="T44" s="49"/>
+      <c r="U44" s="49"/>
+      <c r="V44" s="49"/>
+      <c r="W44" s="49"/>
+      <c r="X44" s="49"/>
+      <c r="Y44" s="49"/>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
         <v>74</v>
@@ -2796,22 +2851,22 @@
         <v>76</v>
       </c>
       <c r="I45" t="s">
-        <v>85</v>
-      </c>
-      <c r="S45" s="54"/>
-      <c r="T45" s="54"/>
-      <c r="U45" s="54"/>
-      <c r="V45" s="54"/>
-      <c r="W45" s="54"/>
-      <c r="X45" s="54"/>
-      <c r="Y45" s="54"/>
+        <v>83</v>
+      </c>
+      <c r="S45" s="49"/>
+      <c r="T45" s="49"/>
+      <c r="U45" s="49"/>
+      <c r="V45" s="49"/>
+      <c r="W45" s="49"/>
+      <c r="X45" s="49"/>
+      <c r="Y45" s="49"/>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
         <v>74</v>
@@ -2826,70 +2881,73 @@
         <v>76</v>
       </c>
       <c r="I46" t="s">
+        <v>85</v>
+      </c>
+      <c r="S46" s="49"/>
+      <c r="T46" s="49"/>
+      <c r="U46" s="49"/>
+      <c r="V46" s="49"/>
+      <c r="W46" s="49"/>
+      <c r="X46" s="49"/>
+      <c r="Y46" s="49"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" t="s">
+        <v>75</v>
+      </c>
+      <c r="F47" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47" t="s">
+        <v>76</v>
+      </c>
+      <c r="I47" t="s">
         <v>86</v>
       </c>
-      <c r="S46" s="54"/>
-      <c r="T46" s="54"/>
-      <c r="U46" s="54"/>
-      <c r="V46" s="54"/>
-      <c r="W46" s="54"/>
-      <c r="X46" s="54"/>
-      <c r="Y46" s="54"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S47" s="54"/>
-      <c r="T47" s="54"/>
-      <c r="U47" s="54"/>
-      <c r="V47" s="54"/>
-      <c r="W47" s="54"/>
-      <c r="X47" s="54"/>
-      <c r="Y47" s="54"/>
+      <c r="S47" s="49"/>
+      <c r="T47" s="49"/>
+      <c r="U47" s="49"/>
+      <c r="V47" s="49"/>
+      <c r="W47" s="49"/>
+      <c r="X47" s="49"/>
+      <c r="Y47" s="49"/>
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I48" t="s">
+      <c r="S48" s="49"/>
+      <c r="T48" s="49"/>
+      <c r="U48" s="49"/>
+      <c r="V48" s="49"/>
+      <c r="W48" s="49"/>
+      <c r="X48" s="49"/>
+      <c r="Y48" s="49"/>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
         <v>114</v>
       </c>
-      <c r="S48" s="54"/>
-      <c r="T48" s="54"/>
-      <c r="U48" s="54"/>
-      <c r="V48" s="54"/>
-      <c r="W48" s="54"/>
-      <c r="X48" s="54"/>
-      <c r="Y48" s="54"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>36</v>
-      </c>
-      <c r="B49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" t="s">
-        <v>89</v>
-      </c>
-      <c r="F49" t="s">
-        <v>119</v>
-      </c>
-      <c r="G49" t="s">
-        <v>76</v>
-      </c>
-      <c r="I49" t="s">
-        <v>92</v>
-      </c>
-      <c r="S49" s="54"/>
-      <c r="T49" s="54"/>
-      <c r="U49" s="54"/>
-      <c r="V49" s="54"/>
-      <c r="W49" s="54"/>
-      <c r="X49" s="54"/>
-      <c r="Y49" s="54"/>
+      <c r="S49" s="49"/>
+      <c r="T49" s="49"/>
+      <c r="U49" s="49"/>
+      <c r="V49" s="49"/>
+      <c r="W49" s="49"/>
+      <c r="X49" s="49"/>
+      <c r="Y49" s="49"/>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C50" t="s">
         <v>89</v>
@@ -2901,29 +2959,26 @@
         <v>76</v>
       </c>
       <c r="I50" t="s">
-        <v>93</v>
-      </c>
-      <c r="S50" s="54"/>
-      <c r="T50" s="54"/>
-      <c r="U50" s="54"/>
-      <c r="V50" s="54"/>
-      <c r="W50" s="54"/>
-      <c r="X50" s="54"/>
-      <c r="Y50" s="54"/>
+        <v>92</v>
+      </c>
+      <c r="S50" s="49"/>
+      <c r="T50" s="49"/>
+      <c r="U50" s="49"/>
+      <c r="V50" s="49"/>
+      <c r="W50" s="49"/>
+      <c r="X50" s="49"/>
+      <c r="Y50" s="49"/>
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C51" t="s">
         <v>89</v>
       </c>
-      <c r="D51" t="s">
-        <v>91</v>
-      </c>
       <c r="F51" t="s">
         <v>119</v>
       </c>
@@ -2931,26 +2986,29 @@
         <v>76</v>
       </c>
       <c r="I51" t="s">
-        <v>94</v>
-      </c>
-      <c r="S51" s="54"/>
-      <c r="T51" s="54"/>
-      <c r="U51" s="54"/>
-      <c r="V51" s="54"/>
-      <c r="W51" s="54"/>
-      <c r="X51" s="54"/>
-      <c r="Y51" s="54"/>
+        <v>93</v>
+      </c>
+      <c r="S51" s="49"/>
+      <c r="T51" s="49"/>
+      <c r="U51" s="49"/>
+      <c r="V51" s="49"/>
+      <c r="W51" s="49"/>
+      <c r="X51" s="49"/>
+      <c r="Y51" s="49"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>163</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>168</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
         <v>89</v>
       </c>
+      <c r="D52" t="s">
+        <v>91</v>
+      </c>
       <c r="F52" t="s">
         <v>119</v>
       </c>
@@ -2958,22 +3016,22 @@
         <v>76</v>
       </c>
       <c r="I52" t="s">
-        <v>162</v>
-      </c>
-      <c r="S52" s="54"/>
-      <c r="T52" s="54"/>
-      <c r="U52" s="54"/>
-      <c r="V52" s="54"/>
-      <c r="W52" s="54"/>
-      <c r="X52" s="54"/>
-      <c r="Y52" s="54"/>
+        <v>94</v>
+      </c>
+      <c r="S52" s="49"/>
+      <c r="T52" s="49"/>
+      <c r="U52" s="49"/>
+      <c r="V52" s="49"/>
+      <c r="W52" s="49"/>
+      <c r="X52" s="49"/>
+      <c r="Y52" s="49"/>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B53" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="C53" t="s">
         <v>89</v>
@@ -2985,70 +3043,70 @@
         <v>76</v>
       </c>
       <c r="I53" t="s">
+        <v>162</v>
+      </c>
+      <c r="S53" s="49"/>
+      <c r="T53" s="49"/>
+      <c r="U53" s="49"/>
+      <c r="V53" s="49"/>
+      <c r="W53" s="49"/>
+      <c r="X53" s="49"/>
+      <c r="Y53" s="49"/>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>165</v>
+      </c>
+      <c r="B54" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F54" t="s">
+        <v>119</v>
+      </c>
+      <c r="G54" t="s">
+        <v>76</v>
+      </c>
+      <c r="I54" t="s">
         <v>167</v>
       </c>
-      <c r="S53" s="54"/>
-      <c r="T53" s="54"/>
-      <c r="U53" s="54"/>
-      <c r="V53" s="54"/>
-      <c r="W53" s="54"/>
-      <c r="X53" s="54"/>
-      <c r="Y53" s="54"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S54" s="54"/>
-      <c r="T54" s="54"/>
-      <c r="U54" s="54"/>
-      <c r="V54" s="54"/>
-      <c r="W54" s="54"/>
-      <c r="X54" s="54"/>
-      <c r="Y54" s="54"/>
+      <c r="S54" s="49"/>
+      <c r="T54" s="49"/>
+      <c r="U54" s="49"/>
+      <c r="V54" s="49"/>
+      <c r="W54" s="49"/>
+      <c r="X54" s="49"/>
+      <c r="Y54" s="49"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="I55" t="s">
+      <c r="S55" s="49"/>
+      <c r="T55" s="49"/>
+      <c r="U55" s="49"/>
+      <c r="V55" s="49"/>
+      <c r="W55" s="49"/>
+      <c r="X55" s="49"/>
+      <c r="Y55" s="49"/>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="I56" t="s">
         <v>115</v>
       </c>
-      <c r="S55" s="54"/>
-      <c r="T55" s="54"/>
-      <c r="U55" s="54"/>
-      <c r="V55" s="54"/>
-      <c r="W55" s="54"/>
-      <c r="X55" s="54"/>
-      <c r="Y55" s="54"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>125</v>
-      </c>
-      <c r="B56" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" t="s">
-        <v>88</v>
-      </c>
-      <c r="F56" t="s">
-        <v>77</v>
-      </c>
-      <c r="G56" t="s">
-        <v>76</v>
-      </c>
-      <c r="I56" t="s">
-        <v>126</v>
-      </c>
-      <c r="S56" s="54"/>
-      <c r="T56" s="54"/>
-      <c r="U56" s="54"/>
-      <c r="V56" s="54"/>
-      <c r="W56" s="54"/>
-      <c r="X56" s="54"/>
-      <c r="Y56" s="54"/>
+      <c r="S56" s="49"/>
+      <c r="T56" s="49"/>
+      <c r="U56" s="49"/>
+      <c r="V56" s="49"/>
+      <c r="W56" s="49"/>
+      <c r="X56" s="49"/>
+      <c r="Y56" s="49"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C57" t="s">
         <v>88</v>
@@ -3060,29 +3118,26 @@
         <v>76</v>
       </c>
       <c r="I57" t="s">
-        <v>95</v>
-      </c>
-      <c r="S57" s="54"/>
-      <c r="T57" s="54"/>
-      <c r="U57" s="54"/>
-      <c r="V57" s="54"/>
-      <c r="W57" s="54"/>
-      <c r="X57" s="54"/>
-      <c r="Y57" s="54"/>
+        <v>126</v>
+      </c>
+      <c r="S57" s="49"/>
+      <c r="T57" s="49"/>
+      <c r="U57" s="49"/>
+      <c r="V57" s="49"/>
+      <c r="W57" s="49"/>
+      <c r="X57" s="49"/>
+      <c r="Y57" s="49"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
         <v>88</v>
       </c>
-      <c r="D58" t="s">
-        <v>91</v>
-      </c>
       <c r="F58" t="s">
         <v>77</v>
       </c>
@@ -3090,26 +3145,29 @@
         <v>76</v>
       </c>
       <c r="I58" t="s">
-        <v>96</v>
-      </c>
-      <c r="S58" s="54"/>
-      <c r="T58" s="54"/>
-      <c r="U58" s="54"/>
-      <c r="V58" s="54"/>
-      <c r="W58" s="54"/>
-      <c r="X58" s="54"/>
-      <c r="Y58" s="54"/>
+        <v>95</v>
+      </c>
+      <c r="S58" s="49"/>
+      <c r="T58" s="49"/>
+      <c r="U58" s="49"/>
+      <c r="V58" s="49"/>
+      <c r="W58" s="49"/>
+      <c r="X58" s="49"/>
+      <c r="Y58" s="49"/>
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>149</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C59" t="s">
         <v>88</v>
       </c>
+      <c r="D59" t="s">
+        <v>91</v>
+      </c>
       <c r="F59" t="s">
         <v>77</v>
       </c>
@@ -3117,22 +3175,22 @@
         <v>76</v>
       </c>
       <c r="I59" t="s">
-        <v>150</v>
-      </c>
-      <c r="S59" s="54"/>
-      <c r="T59" s="54"/>
-      <c r="U59" s="54"/>
-      <c r="V59" s="54"/>
-      <c r="W59" s="54"/>
-      <c r="X59" s="54"/>
-      <c r="Y59" s="54"/>
+        <v>96</v>
+      </c>
+      <c r="S59" s="49"/>
+      <c r="T59" s="49"/>
+      <c r="U59" s="49"/>
+      <c r="V59" s="49"/>
+      <c r="W59" s="49"/>
+      <c r="X59" s="49"/>
+      <c r="Y59" s="49"/>
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B60" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="C60" t="s">
         <v>88</v>
@@ -3144,22 +3202,22 @@
         <v>76</v>
       </c>
       <c r="I60" t="s">
-        <v>161</v>
-      </c>
-      <c r="S60" s="54"/>
-      <c r="T60" s="54"/>
-      <c r="U60" s="54"/>
-      <c r="V60" s="54"/>
-      <c r="W60" s="54"/>
-      <c r="X60" s="54"/>
-      <c r="Y60" s="54"/>
+        <v>150</v>
+      </c>
+      <c r="S60" s="49"/>
+      <c r="T60" s="49"/>
+      <c r="U60" s="49"/>
+      <c r="V60" s="49"/>
+      <c r="W60" s="49"/>
+      <c r="X60" s="49"/>
+      <c r="Y60" s="49"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B61" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="C61" t="s">
         <v>88</v>
@@ -3171,76 +3229,73 @@
         <v>76</v>
       </c>
       <c r="I61" t="s">
+        <v>161</v>
+      </c>
+      <c r="S61" s="49"/>
+      <c r="T61" s="49"/>
+      <c r="U61" s="49"/>
+      <c r="V61" s="49"/>
+      <c r="W61" s="49"/>
+      <c r="X61" s="49"/>
+      <c r="Y61" s="49"/>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62" t="s">
+        <v>88</v>
+      </c>
+      <c r="F62" t="s">
+        <v>77</v>
+      </c>
+      <c r="G62" t="s">
+        <v>76</v>
+      </c>
+      <c r="I62" t="s">
         <v>166</v>
       </c>
-      <c r="S61" s="54"/>
-      <c r="T61" s="54"/>
-      <c r="U61" s="54"/>
-      <c r="V61" s="54"/>
-      <c r="W61" s="54"/>
-      <c r="X61" s="54"/>
-      <c r="Y61" s="54"/>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S62" s="54"/>
-      <c r="T62" s="54"/>
-      <c r="U62" s="54"/>
-      <c r="V62" s="54"/>
-      <c r="W62" s="54"/>
-      <c r="X62" s="54"/>
-      <c r="Y62" s="54"/>
+      <c r="S62" s="49"/>
+      <c r="T62" s="49"/>
+      <c r="U62" s="49"/>
+      <c r="V62" s="49"/>
+      <c r="W62" s="49"/>
+      <c r="X62" s="49"/>
+      <c r="Y62" s="49"/>
     </row>
     <row r="63" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="S63" s="54"/>
-      <c r="T63" s="54"/>
-      <c r="U63" s="54"/>
-      <c r="V63" s="54"/>
-      <c r="W63" s="54"/>
-      <c r="X63" s="54"/>
-      <c r="Y63" s="54"/>
+      <c r="S63" s="49"/>
+      <c r="T63" s="49"/>
+      <c r="U63" s="49"/>
+      <c r="V63" s="49"/>
+      <c r="W63" s="49"/>
+      <c r="X63" s="49"/>
+      <c r="Y63" s="49"/>
     </row>
     <row r="64" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="S64" s="49"/>
+      <c r="T64" s="49"/>
+      <c r="U64" s="49"/>
+      <c r="V64" s="49"/>
+      <c r="W64" s="49"/>
+      <c r="X64" s="49"/>
+      <c r="Y64" s="49"/>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>151</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>88</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>152</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>82</v>
-      </c>
-      <c r="F64" t="s">
-        <v>77</v>
-      </c>
-      <c r="G64" t="s">
-        <v>79</v>
-      </c>
-      <c r="I64" t="s">
-        <v>153</v>
-      </c>
-      <c r="S64" s="54"/>
-      <c r="T64" s="54"/>
-      <c r="U64" s="54"/>
-      <c r="V64" s="54"/>
-      <c r="W64" s="54"/>
-      <c r="X64" s="54"/>
-      <c r="Y64" s="54"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>58</v>
-      </c>
-      <c r="B65" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" t="s">
-        <v>75</v>
-      </c>
-      <c r="D65" t="s">
-        <v>103</v>
       </c>
       <c r="F65" t="s">
         <v>77</v>
@@ -3249,21 +3304,28 @@
         <v>79</v>
       </c>
       <c r="I65" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="S65" s="49"/>
+      <c r="T65" s="49"/>
+      <c r="U65" s="49"/>
+      <c r="V65" s="49"/>
+      <c r="W65" s="49"/>
+      <c r="X65" s="49"/>
+      <c r="Y65" s="49"/>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="D66" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F66" t="s">
         <v>77</v>
@@ -3272,21 +3334,21 @@
         <v>79</v>
       </c>
       <c r="I66" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C67" t="s">
         <v>88</v>
       </c>
       <c r="D67" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="F67" t="s">
         <v>77</v>
@@ -3295,21 +3357,21 @@
         <v>79</v>
       </c>
       <c r="I67" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C68" t="s">
         <v>88</v>
       </c>
       <c r="D68" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
       <c r="F68" t="s">
         <v>77</v>
@@ -3318,15 +3380,15 @@
         <v>79</v>
       </c>
       <c r="I68" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>62</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C69" t="s">
         <v>88</v>
@@ -3341,21 +3403,21 @@
         <v>79</v>
       </c>
       <c r="I69" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>63</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
         <v>88</v>
       </c>
       <c r="D70" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F70" t="s">
         <v>77</v>
@@ -3364,21 +3426,21 @@
         <v>79</v>
       </c>
       <c r="I70" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="C71" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D71" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="F71" t="s">
         <v>77</v>
@@ -3387,52 +3449,52 @@
         <v>79</v>
       </c>
       <c r="I71" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72" t="s">
+        <v>78</v>
+      </c>
+      <c r="F72" t="s">
+        <v>77</v>
+      </c>
+      <c r="G72" t="s">
+        <v>79</v>
+      </c>
+      <c r="I72" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B74" s="53" t="s">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B75" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C74" s="53" t="s">
+      <c r="C75" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="D74" s="53" t="s">
+      <c r="D75" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I75" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>64</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>100</v>
-      </c>
-      <c r="C75" t="s">
-        <v>90</v>
-      </c>
-      <c r="D75" t="s">
-        <v>103</v>
-      </c>
-      <c r="F75" t="s">
-        <v>119</v>
-      </c>
-      <c r="G75" t="s">
-        <v>105</v>
-      </c>
-      <c r="I75" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>67</v>
-      </c>
-      <c r="B76" t="s">
-        <v>89</v>
       </c>
       <c r="C76" t="s">
         <v>90</v>
@@ -3447,15 +3509,15 @@
         <v>105</v>
       </c>
       <c r="I76" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B77" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
         <v>90</v>
@@ -3470,15 +3532,15 @@
         <v>105</v>
       </c>
       <c r="I77" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C78" t="s">
         <v>90</v>
@@ -3493,18 +3555,18 @@
         <v>105</v>
       </c>
       <c r="I78" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B79" t="s">
-        <v>110</v>
+        <v>81</v>
       </c>
       <c r="C79" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D79" t="s">
         <v>103</v>
@@ -3516,15 +3578,15 @@
         <v>105</v>
       </c>
       <c r="I79" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B80" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C80" t="s">
         <v>82</v>
@@ -3539,60 +3601,66 @@
         <v>105</v>
       </c>
       <c r="I80" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B81" t="s">
-        <v>117</v>
+        <v>90</v>
+      </c>
+      <c r="C81" t="s">
+        <v>82</v>
+      </c>
+      <c r="D81" t="s">
+        <v>103</v>
+      </c>
+      <c r="F81" t="s">
+        <v>119</v>
+      </c>
+      <c r="G81" t="s">
+        <v>105</v>
+      </c>
+      <c r="I81" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>69</v>
+      </c>
+      <c r="B82" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>155</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>88</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>78</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>154</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F83" t="s">
         <v>119</v>
       </c>
-      <c r="G82" t="s">
+      <c r="G83" t="s">
         <v>105</v>
       </c>
-      <c r="I82" t="s">
+      <c r="I83" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>71</v>
-      </c>
-      <c r="B85" t="s">
-        <v>110</v>
-      </c>
-      <c r="C85" t="s">
-        <v>81</v>
-      </c>
-      <c r="D85" t="s">
-        <v>82</v>
-      </c>
-      <c r="I85" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B86" t="s">
         <v>110</v>
@@ -3601,40 +3669,57 @@
         <v>81</v>
       </c>
       <c r="D86" t="s">
-        <v>103</v>
-      </c>
-      <c r="E86" t="s">
         <v>82</v>
       </c>
       <c r="I86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>72</v>
+      </c>
+      <c r="B87" t="s">
+        <v>110</v>
+      </c>
+      <c r="C87" t="s">
+        <v>81</v>
+      </c>
+      <c r="D87" t="s">
+        <v>103</v>
+      </c>
+      <c r="E87" t="s">
+        <v>82</v>
+      </c>
+      <c r="I87" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>73</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>121</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>122</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>101</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F88" t="s">
         <v>128</v>
       </c>
-      <c r="G87" t="s">
+      <c r="G88" t="s">
         <v>127</v>
       </c>
-      <c r="I87" t="s">
+      <c r="I88" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B13:M13">
+  <conditionalFormatting sqref="B14:M14">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3646,7 +3731,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:M14">
+  <conditionalFormatting sqref="B15:M15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3658,7 +3743,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:M15">
+  <conditionalFormatting sqref="B16:M16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3696,18 +3781,18 @@
   <sheetData>
     <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="55">
+      <c r="C3" s="53"/>
+      <c r="D3" s="50">
         <f>20*12*4</f>
         <v>960</v>
       </c>
@@ -3727,11 +3812,11 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="57">
+      <c r="C5" s="52">
         <f>POWER($D$3,1 + B5 *0.1)</f>
         <v>960</v>
       </c>
-      <c r="D5" s="56">
+      <c r="D5" s="51">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>0.8</v>
       </c>
@@ -3740,11 +3825,11 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="57">
+      <c r="C6" s="52">
         <f t="shared" ref="C6:C14" si="0">POWER($D$3,1 + B6 *0.15)</f>
         <v>7532.7335020499258</v>
       </c>
-      <c r="D6" s="56">
+      <c r="D6" s="51">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>6.2772779183749376</v>
       </c>
@@ -3753,11 +3838,11 @@
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="57">
+      <c r="C7" s="52">
         <f t="shared" si="0"/>
         <v>59106.327096776331</v>
       </c>
-      <c r="D7" s="56">
+      <c r="D7" s="51">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>49.255272580646945</v>
       </c>
@@ -3766,11 +3851,11 @@
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="57">
+      <c r="C8" s="52">
         <f t="shared" si="0"/>
         <v>463783.55240104912</v>
       </c>
-      <c r="D8" s="56">
+      <c r="D8" s="51">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>386.48629366754091</v>
       </c>
@@ -3779,11 +3864,11 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="57">
+      <c r="C9" s="52">
         <f t="shared" si="0"/>
         <v>3639122.8154907427</v>
       </c>
-      <c r="D9" s="56">
+      <c r="D9" s="51">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>3032.6023462422859</v>
       </c>
@@ -3792,11 +3877,11 @@
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" s="57">
+      <c r="C10" s="52">
         <f t="shared" si="0"/>
         <v>10193830.257075245</v>
       </c>
-      <c r="D10" s="56">
+      <c r="D10" s="51">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>8494.8585475627042</v>
       </c>
@@ -3805,11 +3890,11 @@
       <c r="B11">
         <v>19</v>
       </c>
-      <c r="C11" s="57">
+      <c r="C11" s="52">
         <f t="shared" si="0"/>
         <v>303210507415.43286</v>
       </c>
-      <c r="D11" s="56">
+      <c r="D11" s="51">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>252675422.84619406</v>
       </c>
@@ -3818,37 +3903,37 @@
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="57">
+      <c r="C12" s="52">
         <f t="shared" si="0"/>
         <v>79986881.970500872</v>
       </c>
-      <c r="D12" s="56">
+      <c r="D12" s="51">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>66655.734975417392</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="59">
+      <c r="B13" s="54">
         <v>12</v>
       </c>
-      <c r="C13" s="60">
+      <c r="C13" s="55">
         <f t="shared" si="0"/>
         <v>224057482.78930962</v>
       </c>
-      <c r="D13" s="61">
+      <c r="D13" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>186714.56899109136</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="59">
+      <c r="B14" s="54">
         <v>15</v>
       </c>
-      <c r="C14" s="60">
+      <c r="C14" s="55">
         <f t="shared" si="0"/>
         <v>4924719592.9163141</v>
       </c>
-      <c r="D14" s="61">
+      <c r="D14" s="56">
         <f>Tabelle2[[#This Row],[Duration (ticks)]]/20/60</f>
         <v>4103932.9940969283</v>
       </c>

</xml_diff>